<commit_message>
fixed the land and water distrib. table option crashing.
</commit_message>
<xml_diff>
--- a/file template.xlsx
+++ b/file template.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Giuliano\Documents\USB BACKUP\TESTGAME\2-11-2015\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Giuliano\Documents\RFWG\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="5955" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="5955" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="world_hydro" sheetId="4" r:id="rId1"/>
     <sheet name="landandwater_distro" sheetId="5" r:id="rId2"/>
     <sheet name="Sheet4" sheetId="7" r:id="rId3"/>
     <sheet name="worldsize" sheetId="2" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId5"/>
-    <sheet name="worldhook" sheetId="1" r:id="rId6"/>
+    <sheet name="worldhook" sheetId="1" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">worldhook!$A$2:$N$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">worldhook!$A$2:$N$2</definedName>
   </definedNames>
-  <calcPr calcId="152511" iterate="1"/>
+  <calcPr calcId="171027" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="362">
   <si>
     <t>Aerial</t>
   </si>
@@ -970,160 +970,160 @@
     <t>--[[[Planetary Diameter]]]--</t>
   </si>
   <si>
-    <t>landandwater_distro</t>
-  </si>
-  <si>
-    <t>landandwater_distro[1] = {createworldcode = 0, text = "--[[[Regional Land &amp; Water Distribution]]]--",x =755,y = 30}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[2] = {createworldcode = 0, text = "World Hydrographic Percentage",x =755,y = 45}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[3] = {createworldcode = 1, text = "Water",x =755,y = 60}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[4] = {createworldcode = 2, text = "Water w/ Minor Islands",x =755,y = 75}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[5] = {createworldcode = 3, text = "Water w/ Major Islands",x =755,y = 90}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[6] = {createworldcode = 4, text = "Water and Land",x =755,y = 105}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[7] = {createworldcode = 5, text = "Land w/ Major Seas",x =755,y = 120}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[8] = {createworldcode = 6, text = "Land w/ Minor Lakes or Seas",x =755,y = 135}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[9] = {createworldcode = 7, text = "Land",x =755,y = 150}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[10] = {createworldcode = 8, text = "20%",x =755,y = 30}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[11] = {createworldcode = 9, text = "0",x =755,y = 45}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[12] = {createworldcode = 10, text = "0",x =755,y = 60}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[13] = {createworldcode = 11, text = "0",x =755,y = 75}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[14] = {createworldcode = 12, text = "2",x =755,y = 90}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[15] = {createworldcode = 13, text = "6",x =755,y = 105}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[16] = {createworldcode = 14, text = "4",x =755,y = 120}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[17] = {createworldcode = 15, text = "8",x =755,y = 135}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[18] = {createworldcode = 16, text = "40%",x =855,y = 30}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[19] = {createworldcode = 17, text = "0",x =855,y = 45}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[20] = {createworldcode = 18, text = "1",x =855,y = 60}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[21] = {createworldcode = 19, text = "4",x =855,y = 75}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[22] = {createworldcode = 20, text = "4",x =855,y = 90}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[23] = {createworldcode = 21, text = "3",x =855,y = 105}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[24] = {createworldcode = 22, text = "3",x =855,y = 120}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[25] = {createworldcode = 23, text = "5",x =855,y = 135}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[26] = {createworldcode = 24, text = "60%",x =955,y = 30}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[27] = {createworldcode = 25, text = "2",x =955,y = 45}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[28] = {createworldcode = 26, text = "4",x =955,y = 60}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[29] = {createworldcode = 27, text = "5",x =955,y = 75}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[30] = {createworldcode = 28, text = "4",x =955,y = 90}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[31] = {createworldcode = 29, text = "3",x =955,y = 105}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[32] = {createworldcode = 30, text = "2",x =955,y = 120}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[33] = {createworldcode = 31, text = "0",x =955,y = 135}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[34] = {createworldcode = 32, text = "80%",x =1055,y = 30}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[35] = {createworldcode = 33, text = "8",x =1055,y = 45}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[36] = {createworldcode = 34, text = "6",x =1055,y = 60}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[37] = {createworldcode = 35, text = "4",x =1055,y = 75}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[38] = {createworldcode = 36, text = "2",x =1055,y = 90}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[39] = {createworldcode = 37, text = "0",x =1055,y = 105}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[40] = {createworldcode = 38, text = "0",x =1055,y = 120}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[41] = {createworldcode = 39, text = "0",x =1055,y = 135}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[42] = {createworldcode = 40, text = "100%",x =1155,y = 30}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[43] = {createworldcode = 41, text = "18",x =1155,y = 45}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[44] = {createworldcode = 42, text = "2",x =1155,y = 60}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[45] = {createworldcode = 43, text = "0",x =1155,y = 75}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[46] = {createworldcode = 44, text = "0",x =1155,y = 90}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[47] = {createworldcode = 45, text = "0",x =1155,y = 105}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[48] = {createworldcode = 46, text = "0",x =1155,y = 120}</t>
-  </si>
-  <si>
-    <t>landandwater_distro[49] = {createworldcode = 47, text = "0",x =1155,y = 135}</t>
+    <t>landandwaterdistro</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[1] = {createworldcode = 0, text = "--[[[Regional Land &amp; Water Distribution]]]--",x =755,y = 30}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[13] = {createworldcode = 11, text = "0",x =755,y = 90}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[21] = {createworldcode = 19, text = "4",x =855,y = 90}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[29] = {createworldcode = 27, text = "5",x =955,y = 90}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[37] = {createworldcode = 35, text = "4",x =1055,y = 90}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[45] = {createworldcode = 43, text = "0",x =1155,y = 90}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[2] = {createworldcode = 0, text = "World Hydrographic Percentage",x =755,y = 45}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[3] = {createworldcode = 1, text = "Water",x =755,y = 60}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[4] = {createworldcode = 2, text = "Water w/ Minor Islands",x =755,y = 75}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[5] = {createworldcode = 3, text = "Water w/ Major Islands",x =755,y = 90}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[6] = {createworldcode = 4, text = "Water and Land",x =755,y = 105}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[7] = {createworldcode = 5, text = "Land w/ Major Seas",x =755,y = 120}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[8] = {createworldcode = 6, text = "Land w/ Minor Lakes or Seas",x =755,y = 135}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[9] = {createworldcode = 7, text = "Land",x =755,y = 150}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[10] = {createworldcode = 8, text = "20%",x =755,y = 45}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[11] = {createworldcode = 9, text = "0",x =755,y = 60}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[12] = {createworldcode = 10, text = "0",x =755,y = 75}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[14] = {createworldcode = 12, text = "2",x =755,y = 105}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[15] = {createworldcode = 13, text = "6",x =755,y = 120}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[16] = {createworldcode = 14, text = "4",x =755,y = 135}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[17] = {createworldcode = 15, text = "8",x =755,y = 150}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[18] = {createworldcode = 16, text = "40%",x =855,y = 45}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[19] = {createworldcode = 17, text = "0",x =855,y = 60}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[20] = {createworldcode = 18, text = "1",x =855,y = 75}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[22] = {createworldcode = 20, text = "4",x =855,y = 105}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[23] = {createworldcode = 21, text = "3",x =855,y = 120}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[24] = {createworldcode = 22, text = "3",x =855,y = 135}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[25] = {createworldcode = 23, text = "5",x =855,y = 150}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[26] = {createworldcode = 24, text = "60%",x =955,y = 45}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[27] = {createworldcode = 25, text = "2",x =955,y = 60}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[28] = {createworldcode = 26, text = "4",x =955,y = 75}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[30] = {createworldcode = 28, text = "4",x =955,y = 105}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[31] = {createworldcode = 29, text = "3",x =955,y = 120}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[32] = {createworldcode = 30, text = "2",x =955,y = 135}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[33] = {createworldcode = 31, text = "0",x =955,y = 150}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[34] = {createworldcode = 32, text = "80%",x =1055,y = 45}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[35] = {createworldcode = 33, text = "8",x =1055,y = 60}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[36] = {createworldcode = 34, text = "6",x =1055,y = 75}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[38] = {createworldcode = 36, text = "2",x =1055,y = 105}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[39] = {createworldcode = 37, text = "0",x =1055,y = 120}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[40] = {createworldcode = 38, text = "0",x =1055,y = 135}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[41] = {createworldcode = 39, text = "0",x =1055,y = 150}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[42] = {createworldcode = 40, text = "100%",x =1155,y = 45}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[43] = {createworldcode = 41, text = "18",x =1155,y = 60}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[44] = {createworldcode = 42, text = "2",x =1155,y = 75}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[46] = {createworldcode = 44, text = "0",x =1155,y = 105}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[47] = {createworldcode = 45, text = "0",x =1155,y = 120}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[48] = {createworldcode = 46, text = "0",x =1155,y = 135}</t>
+  </si>
+  <si>
+    <t>landandwaterdistro[49] = {createworldcode = 47, text = "0",x =1155,y = 150}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1277,6 +1277,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1312,6 +1329,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1467,23 +1501,22 @@
   <dimension ref="A1:N51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="1.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="50.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="3.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="1.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="59.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="11" width="8.85546875" style="4"/>
-    <col min="12" max="12" width="50.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="60.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.85546875" style="4"/>
-    <col min="14" max="14" width="2.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="15" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
@@ -1589,7 +1622,7 @@
         <v>755</v>
       </c>
       <c r="E5" s="4">
-        <f t="shared" ref="E5:E14" si="2">E4+$E$1</f>
+        <f>E4+$E$1</f>
         <v>60</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -1621,7 +1654,7 @@
         <v>755</v>
       </c>
       <c r="E6" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="E5:E14" si="2">E5+$E$1</f>
         <v>75</v>
       </c>
       <c r="F6" s="5" t="s">
@@ -2082,8 +2115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3:L51"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2095,8 +2128,8 @@
     <col min="5" max="5" width="3.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="1.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="69.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="60.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="73.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="73.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -2164,7 +2197,7 @@
       </c>
       <c r="H3" s="4" t="str">
         <f>CONCATENATE($C$1,A3," = ","{",$B$2," = ",B3,", ",$C$2," = ",G3,",",$D$2,D3,",",$E$2,E3,"}","")</f>
-        <v>landandwater_distro[1] = {createworldcode = 0, text = "--[[[Regional Land &amp; Water Distribution]]]--",x =755,y = 30}</v>
+        <v>landandwaterdistro[1] = {createworldcode = 0, text = "--[[[Regional Land &amp; Water Distribution]]]--",x =755,y = 30}</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
@@ -2194,18 +2227,18 @@
         <v>127</v>
       </c>
       <c r="G4" s="5" t="str">
-        <f t="shared" ref="G4:G14" si="0">CONCATENATE(F4,C4,F4)</f>
+        <f t="shared" ref="G4:G13" si="0">CONCATENATE(F4,C4,F4)</f>
         <v>"World Hydrographic Percentage"</v>
       </c>
       <c r="H4" s="4" t="str">
-        <f t="shared" ref="H4:H14" si="1">CONCATENATE($C$1,A4," = ","{",$B$2," = ",B4,", ",$C$2," = ",G4,",",$D$2,D4,",",$E$2,E4,"}","")</f>
-        <v>landandwater_distro[2] = {createworldcode = 0, text = "World Hydrographic Percentage",x =755,y = 45}</v>
+        <f t="shared" ref="H4:H13" si="1">CONCATENATE($C$1,A4," = ","{",$B$2," = ",B4,", ",$C$2," = ",G4,",",$D$2,D4,",",$E$2,E4,"}","")</f>
+        <v>landandwaterdistro[2] = {createworldcode = 0, text = "World Hydrographic Percentage",x =755,y = 45}</v>
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -2234,13 +2267,13 @@
       </c>
       <c r="H5" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>landandwater_distro[3] = {createworldcode = 1, text = "Water",x =755,y = 60}</v>
+        <v>landandwaterdistro[3] = {createworldcode = 1, text = "Water",x =755,y = 60}</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -2269,13 +2302,13 @@
       </c>
       <c r="H6" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>landandwater_distro[4] = {createworldcode = 2, text = "Water w/ Minor Islands",x =755,y = 75}</v>
+        <v>landandwaterdistro[4] = {createworldcode = 2, text = "Water w/ Minor Islands",x =755,y = 75}</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -2304,13 +2337,13 @@
       </c>
       <c r="H7" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>landandwater_distro[5] = {createworldcode = 3, text = "Water w/ Major Islands",x =755,y = 90}</v>
+        <v>landandwaterdistro[5] = {createworldcode = 3, text = "Water w/ Major Islands",x =755,y = 90}</v>
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -2339,13 +2372,13 @@
       </c>
       <c r="H8" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>landandwater_distro[6] = {createworldcode = 4, text = "Water and Land",x =755,y = 105}</v>
+        <v>landandwaterdistro[6] = {createworldcode = 4, text = "Water and Land",x =755,y = 105}</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -2374,13 +2407,13 @@
       </c>
       <c r="H9" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>landandwater_distro[7] = {createworldcode = 5, text = "Land w/ Major Seas",x =755,y = 120}</v>
+        <v>landandwaterdistro[7] = {createworldcode = 5, text = "Land w/ Major Seas",x =755,y = 120}</v>
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -2409,13 +2442,13 @@
       </c>
       <c r="H10" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>landandwater_distro[8] = {createworldcode = 6, text = "Land w/ Minor Lakes or Seas",x =755,y = 135}</v>
+        <v>landandwaterdistro[8] = {createworldcode = 6, text = "Land w/ Minor Lakes or Seas",x =755,y = 135}</v>
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2444,13 +2477,13 @@
       </c>
       <c r="H11" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>landandwater_distro[9] = {createworldcode = 7, text = "Land",x =755,y = 150}</v>
+        <v>landandwaterdistro[9] = {createworldcode = 7, text = "Land",x =755,y = 150}</v>
       </c>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -2467,7 +2500,8 @@
         <v>755</v>
       </c>
       <c r="E12" s="4">
-        <v>30</v>
+        <f>E3+$E$1</f>
+        <v>45</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>127</v>
@@ -2478,13 +2512,13 @@
       </c>
       <c r="H12" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>landandwater_distro[10] = {createworldcode = 8, text = "20%",x =755,y = 30}</v>
+        <v>landandwaterdistro[10] = {createworldcode = 8, text = "20%",x =755,y = 45}</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -2502,7 +2536,7 @@
       </c>
       <c r="E13" s="4">
         <f>E12+$E$1</f>
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>127</v>
@@ -2513,13 +2547,13 @@
       </c>
       <c r="H13" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>landandwater_distro[11] = {createworldcode = 9, text = "0",x =755,y = 45}</v>
+        <v>landandwaterdistro[11] = {createworldcode = 9, text = "0",x =755,y = 60}</v>
       </c>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2536,8 +2570,8 @@
         <v>755</v>
       </c>
       <c r="E14" s="4">
-        <f t="shared" si="2"/>
-        <v>60</v>
+        <f>E13+$E$1</f>
+        <v>75</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>127</v>
@@ -2548,13 +2582,13 @@
       </c>
       <c r="H14" s="4" t="str">
         <f>CONCATENATE($C$1,A14," = ","{",$B$2," = ",B14,", ",$C$2," = ",G14,",",$D$2,D14,",",$E$2,E14,"}","")</f>
-        <v>landandwater_distro[12] = {createworldcode = 10, text = "0",x =755,y = 60}</v>
+        <v>landandwaterdistro[12] = {createworldcode = 10, text = "0",x =755,y = 75}</v>
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4" t="s">
-        <v>324</v>
+        <v>329</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2571,8 +2605,8 @@
         <v>755</v>
       </c>
       <c r="E15" s="4">
-        <f t="shared" si="2"/>
-        <v>75</v>
+        <f>E14+$E$1</f>
+        <v>90</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>127</v>
@@ -2583,10 +2617,10 @@
       </c>
       <c r="H15" s="4" t="str">
         <f t="shared" ref="H15:H51" si="4">CONCATENATE($C$1,A15," = ","{",$B$2," = ",B15,", ",$C$2," = ",G15,",",$D$2,D15,",",$E$2,E15,"}","")</f>
-        <v>landandwater_distro[13] = {createworldcode = 11, text = "0",x =755,y = 75}</v>
+        <v>landandwaterdistro[13] = {createworldcode = 11, text = "0",x =755,y = 90}</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -2603,8 +2637,8 @@
         <v>755</v>
       </c>
       <c r="E16" s="4">
-        <f t="shared" si="2"/>
-        <v>90</v>
+        <f t="shared" ref="E14:E19" si="5">E15+$E$1</f>
+        <v>105</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>127</v>
@@ -2615,10 +2649,10 @@
       </c>
       <c r="H16" s="4" t="str">
         <f>CONCATENATE($C$1,A16," = ","{",$B$2," = ",B16,", ",$C$2," = ",G16,",",$D$2,D16,",",$E$2,E16,"}","")</f>
-        <v>landandwater_distro[14] = {createworldcode = 12, text = "2",x =755,y = 90}</v>
+        <v>landandwaterdistro[14] = {createworldcode = 12, text = "2",x =755,y = 105}</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -2635,8 +2669,8 @@
         <v>755</v>
       </c>
       <c r="E17" s="4">
-        <f t="shared" si="2"/>
-        <v>105</v>
+        <f t="shared" si="5"/>
+        <v>120</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>127</v>
@@ -2647,10 +2681,10 @@
       </c>
       <c r="H17" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>landandwater_distro[15] = {createworldcode = 13, text = "6",x =755,y = 105}</v>
+        <v>landandwaterdistro[15] = {createworldcode = 13, text = "6",x =755,y = 120}</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -2667,8 +2701,8 @@
         <v>755</v>
       </c>
       <c r="E18" s="4">
-        <f t="shared" si="2"/>
-        <v>120</v>
+        <f t="shared" si="5"/>
+        <v>135</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>127</v>
@@ -2679,10 +2713,10 @@
       </c>
       <c r="H18" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>landandwater_distro[16] = {createworldcode = 14, text = "4",x =755,y = 120}</v>
+        <v>landandwaterdistro[16] = {createworldcode = 14, text = "4",x =755,y = 135}</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -2699,8 +2733,8 @@
         <v>755</v>
       </c>
       <c r="E19" s="4">
-        <f t="shared" si="2"/>
-        <v>135</v>
+        <f t="shared" si="5"/>
+        <v>150</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>127</v>
@@ -2711,10 +2745,10 @@
       </c>
       <c r="H19" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>landandwater_distro[17] = {createworldcode = 15, text = "8",x =755,y = 135}</v>
+        <v>landandwaterdistro[17] = {createworldcode = 15, text = "8",x =755,y = 150}</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -2731,7 +2765,8 @@
         <v>855</v>
       </c>
       <c r="E20" s="4">
-        <v>30</v>
+        <f>E3+$E$1</f>
+        <v>45</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>127</v>
@@ -2742,10 +2777,10 @@
       </c>
       <c r="H20" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>landandwater_distro[18] = {createworldcode = 16, text = "40%",x =855,y = 30}</v>
+        <v>landandwaterdistro[18] = {createworldcode = 16, text = "40%",x =855,y = 45}</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -2763,7 +2798,7 @@
       </c>
       <c r="E21" s="4">
         <f>E20+$E$1</f>
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>127</v>
@@ -2774,10 +2809,10 @@
       </c>
       <c r="H21" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>landandwater_distro[19] = {createworldcode = 17, text = "0",x =855,y = 45}</v>
+        <v>landandwaterdistro[19] = {createworldcode = 17, text = "0",x =855,y = 60}</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -2794,8 +2829,8 @@
         <v>855</v>
       </c>
       <c r="E22" s="4">
-        <f t="shared" si="2"/>
-        <v>60</v>
+        <f>E21+$E$1</f>
+        <v>75</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>127</v>
@@ -2806,10 +2841,10 @@
       </c>
       <c r="H22" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>landandwater_distro[20] = {createworldcode = 18, text = "1",x =855,y = 60}</v>
+        <v>landandwaterdistro[20] = {createworldcode = 18, text = "1",x =855,y = 75}</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -2827,7 +2862,7 @@
       </c>
       <c r="E23" s="4">
         <f t="shared" si="2"/>
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>127</v>
@@ -2838,10 +2873,10 @@
       </c>
       <c r="H23" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>landandwater_distro[21] = {createworldcode = 19, text = "4",x =855,y = 75}</v>
+        <v>landandwaterdistro[21] = {createworldcode = 19, text = "4",x =855,y = 90}</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>333</v>
+        <v>315</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -2859,7 +2894,7 @@
       </c>
       <c r="E24" s="4">
         <f t="shared" si="2"/>
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>127</v>
@@ -2870,10 +2905,10 @@
       </c>
       <c r="H24" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>landandwater_distro[22] = {createworldcode = 20, text = "4",x =855,y = 90}</v>
+        <v>landandwaterdistro[22] = {createworldcode = 20, text = "4",x =855,y = 105}</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -2891,7 +2926,7 @@
       </c>
       <c r="E25" s="4">
         <f t="shared" si="2"/>
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>127</v>
@@ -2902,10 +2937,10 @@
       </c>
       <c r="H25" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>landandwater_distro[23] = {createworldcode = 21, text = "3",x =855,y = 105}</v>
+        <v>landandwaterdistro[23] = {createworldcode = 21, text = "3",x =855,y = 120}</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -2923,7 +2958,7 @@
       </c>
       <c r="E26" s="4">
         <f t="shared" si="2"/>
-        <v>120</v>
+        <v>135</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>127</v>
@@ -2934,10 +2969,10 @@
       </c>
       <c r="H26" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>landandwater_distro[24] = {createworldcode = 22, text = "3",x =855,y = 120}</v>
+        <v>landandwaterdistro[24] = {createworldcode = 22, text = "3",x =855,y = 135}</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -2955,7 +2990,7 @@
       </c>
       <c r="E27" s="4">
         <f t="shared" si="2"/>
-        <v>135</v>
+        <v>150</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>127</v>
@@ -2966,10 +3001,10 @@
       </c>
       <c r="H27" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>landandwater_distro[25] = {createworldcode = 23, text = "5",x =855,y = 135}</v>
+        <v>landandwaterdistro[25] = {createworldcode = 23, text = "5",x =855,y = 150}</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -2986,7 +3021,8 @@
         <v>955</v>
       </c>
       <c r="E28" s="4">
-        <v>30</v>
+        <f>E3+$E$1</f>
+        <v>45</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>127</v>
@@ -2997,10 +3033,10 @@
       </c>
       <c r="H28" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>landandwater_distro[26] = {createworldcode = 24, text = "60%",x =955,y = 30}</v>
+        <v>landandwaterdistro[26] = {createworldcode = 24, text = "60%",x =955,y = 45}</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -3018,7 +3054,7 @@
       </c>
       <c r="E29" s="4">
         <f>E28+$E$1</f>
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>127</v>
@@ -3029,10 +3065,10 @@
       </c>
       <c r="H29" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>landandwater_distro[27] = {createworldcode = 25, text = "2",x =955,y = 45}</v>
+        <v>landandwaterdistro[27] = {createworldcode = 25, text = "2",x =955,y = 60}</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -3049,8 +3085,8 @@
         <v>955</v>
       </c>
       <c r="E30" s="4">
-        <f t="shared" ref="E30:E35" si="5">E29+$E$1</f>
-        <v>60</v>
+        <f t="shared" ref="E30:E35" si="6">E29+$E$1</f>
+        <v>75</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>127</v>
@@ -3061,10 +3097,10 @@
       </c>
       <c r="H30" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>landandwater_distro[28] = {createworldcode = 26, text = "4",x =955,y = 60}</v>
+        <v>landandwaterdistro[28] = {createworldcode = 26, text = "4",x =955,y = 75}</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -3081,8 +3117,8 @@
         <v>955</v>
       </c>
       <c r="E31" s="4">
-        <f t="shared" si="5"/>
-        <v>75</v>
+        <f t="shared" si="6"/>
+        <v>90</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>127</v>
@@ -3093,10 +3129,10 @@
       </c>
       <c r="H31" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>landandwater_distro[29] = {createworldcode = 27, text = "5",x =955,y = 75}</v>
+        <v>landandwaterdistro[29] = {createworldcode = 27, text = "5",x =955,y = 90}</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>341</v>
+        <v>316</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -3113,8 +3149,8 @@
         <v>955</v>
       </c>
       <c r="E32" s="4">
-        <f t="shared" si="5"/>
-        <v>90</v>
+        <f t="shared" si="6"/>
+        <v>105</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>127</v>
@@ -3125,10 +3161,10 @@
       </c>
       <c r="H32" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>landandwater_distro[30] = {createworldcode = 28, text = "4",x =955,y = 90}</v>
+        <v>landandwaterdistro[30] = {createworldcode = 28, text = "4",x =955,y = 105}</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -3145,8 +3181,8 @@
         <v>955</v>
       </c>
       <c r="E33" s="4">
-        <f t="shared" si="5"/>
-        <v>105</v>
+        <f t="shared" si="6"/>
+        <v>120</v>
       </c>
       <c r="F33" s="5" t="s">
         <v>127</v>
@@ -3157,10 +3193,10 @@
       </c>
       <c r="H33" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>landandwater_distro[31] = {createworldcode = 29, text = "3",x =955,y = 105}</v>
+        <v>landandwaterdistro[31] = {createworldcode = 29, text = "3",x =955,y = 120}</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -3177,8 +3213,8 @@
         <v>955</v>
       </c>
       <c r="E34" s="4">
-        <f t="shared" si="5"/>
-        <v>120</v>
+        <f t="shared" si="6"/>
+        <v>135</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>127</v>
@@ -3189,13 +3225,13 @@
       </c>
       <c r="H34" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>landandwater_distro[32] = {createworldcode = 30, text = "2",x =955,y = 120}</v>
+        <v>landandwaterdistro[32] = {createworldcode = 30, text = "2",x =955,y = 135}</v>
       </c>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
       <c r="L34" s="4" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -3212,8 +3248,8 @@
         <v>955</v>
       </c>
       <c r="E35" s="4">
-        <f t="shared" si="5"/>
-        <v>135</v>
+        <f t="shared" si="6"/>
+        <v>150</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>127</v>
@@ -3224,13 +3260,13 @@
       </c>
       <c r="H35" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>landandwater_distro[33] = {createworldcode = 31, text = "0",x =955,y = 135}</v>
+        <v>landandwaterdistro[33] = {createworldcode = 31, text = "0",x =955,y = 150}</v>
       </c>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
       <c r="L35" s="4" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -3247,7 +3283,8 @@
         <v>1055</v>
       </c>
       <c r="E36" s="4">
-        <v>30</v>
+        <f>E3+$E$1</f>
+        <v>45</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>127</v>
@@ -3258,10 +3295,10 @@
       </c>
       <c r="H36" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>landandwater_distro[34] = {createworldcode = 32, text = "80%",x =1055,y = 30}</v>
+        <v>landandwaterdistro[34] = {createworldcode = 32, text = "80%",x =1055,y = 45}</v>
       </c>
       <c r="L36" s="4" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -3279,7 +3316,7 @@
       </c>
       <c r="E37" s="4">
         <f>E36+$E$1</f>
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="F37" s="5" t="s">
         <v>127</v>
@@ -3290,10 +3327,10 @@
       </c>
       <c r="H37" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>landandwater_distro[35] = {createworldcode = 33, text = "8",x =1055,y = 45}</v>
+        <v>landandwaterdistro[35] = {createworldcode = 33, text = "8",x =1055,y = 60}</v>
       </c>
       <c r="L37" s="4" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -3310,8 +3347,8 @@
         <v>1055</v>
       </c>
       <c r="E38" s="4">
-        <f t="shared" ref="E38:E43" si="6">E37+$E$1</f>
-        <v>60</v>
+        <f t="shared" ref="E38:E43" si="7">E37+$E$1</f>
+        <v>75</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>127</v>
@@ -3322,10 +3359,10 @@
       </c>
       <c r="H38" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>landandwater_distro[36] = {createworldcode = 34, text = "6",x =1055,y = 60}</v>
+        <v>landandwaterdistro[36] = {createworldcode = 34, text = "6",x =1055,y = 75}</v>
       </c>
       <c r="L38" s="4" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -3342,8 +3379,8 @@
         <v>1055</v>
       </c>
       <c r="E39" s="4">
-        <f t="shared" si="6"/>
-        <v>75</v>
+        <f t="shared" si="7"/>
+        <v>90</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>127</v>
@@ -3354,10 +3391,10 @@
       </c>
       <c r="H39" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>landandwater_distro[37] = {createworldcode = 35, text = "4",x =1055,y = 75}</v>
+        <v>landandwaterdistro[37] = {createworldcode = 35, text = "4",x =1055,y = 90}</v>
       </c>
       <c r="L39" s="4" t="s">
-        <v>349</v>
+        <v>317</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
@@ -3374,8 +3411,8 @@
         <v>1055</v>
       </c>
       <c r="E40" s="4">
-        <f t="shared" si="6"/>
-        <v>90</v>
+        <f t="shared" si="7"/>
+        <v>105</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>127</v>
@@ -3386,10 +3423,10 @@
       </c>
       <c r="H40" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>landandwater_distro[38] = {createworldcode = 36, text = "2",x =1055,y = 90}</v>
+        <v>landandwaterdistro[38] = {createworldcode = 36, text = "2",x =1055,y = 105}</v>
       </c>
       <c r="L40" s="4" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
@@ -3406,8 +3443,8 @@
         <v>1055</v>
       </c>
       <c r="E41" s="4">
-        <f t="shared" si="6"/>
-        <v>105</v>
+        <f t="shared" si="7"/>
+        <v>120</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>127</v>
@@ -3418,10 +3455,10 @@
       </c>
       <c r="H41" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>landandwater_distro[39] = {createworldcode = 37, text = "0",x =1055,y = 105}</v>
+        <v>landandwaterdistro[39] = {createworldcode = 37, text = "0",x =1055,y = 120}</v>
       </c>
       <c r="L41" s="4" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
@@ -3438,8 +3475,8 @@
         <v>1055</v>
       </c>
       <c r="E42" s="4">
-        <f t="shared" si="6"/>
-        <v>120</v>
+        <f t="shared" si="7"/>
+        <v>135</v>
       </c>
       <c r="F42" s="5" t="s">
         <v>127</v>
@@ -3450,10 +3487,10 @@
       </c>
       <c r="H42" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>landandwater_distro[40] = {createworldcode = 38, text = "0",x =1055,y = 120}</v>
+        <v>landandwaterdistro[40] = {createworldcode = 38, text = "0",x =1055,y = 135}</v>
       </c>
       <c r="L42" s="4" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
@@ -3470,8 +3507,8 @@
         <v>1055</v>
       </c>
       <c r="E43" s="4">
-        <f t="shared" si="6"/>
-        <v>135</v>
+        <f t="shared" si="7"/>
+        <v>150</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>127</v>
@@ -3482,10 +3519,10 @@
       </c>
       <c r="H43" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>landandwater_distro[41] = {createworldcode = 39, text = "0",x =1055,y = 135}</v>
+        <v>landandwaterdistro[41] = {createworldcode = 39, text = "0",x =1055,y = 150}</v>
       </c>
       <c r="L43" s="4" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
@@ -3502,7 +3539,8 @@
         <v>1155</v>
       </c>
       <c r="E44" s="4">
-        <v>30</v>
+        <f>E3+$E$1</f>
+        <v>45</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>127</v>
@@ -3513,10 +3551,10 @@
       </c>
       <c r="H44" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>landandwater_distro[42] = {createworldcode = 40, text = "100%",x =1155,y = 30}</v>
+        <v>landandwaterdistro[42] = {createworldcode = 40, text = "100%",x =1155,y = 45}</v>
       </c>
       <c r="L44" s="4" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
@@ -3534,7 +3572,7 @@
       </c>
       <c r="E45" s="4">
         <f>E44+$E$1</f>
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>127</v>
@@ -3545,10 +3583,10 @@
       </c>
       <c r="H45" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>landandwater_distro[43] = {createworldcode = 41, text = "18",x =1155,y = 45}</v>
+        <v>landandwaterdistro[43] = {createworldcode = 41, text = "18",x =1155,y = 60}</v>
       </c>
       <c r="L45" s="4" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
@@ -3565,8 +3603,8 @@
         <v>1155</v>
       </c>
       <c r="E46" s="4">
-        <f t="shared" ref="E46:E51" si="7">E45+$E$1</f>
-        <v>60</v>
+        <f t="shared" ref="E46:E51" si="8">E45+$E$1</f>
+        <v>75</v>
       </c>
       <c r="F46" s="5" t="s">
         <v>127</v>
@@ -3577,10 +3615,10 @@
       </c>
       <c r="H46" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>landandwater_distro[44] = {createworldcode = 42, text = "2",x =1155,y = 60}</v>
+        <v>landandwaterdistro[44] = {createworldcode = 42, text = "2",x =1155,y = 75}</v>
       </c>
       <c r="L46" s="4" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
@@ -3597,8 +3635,8 @@
         <v>1155</v>
       </c>
       <c r="E47" s="4">
-        <f t="shared" si="7"/>
-        <v>75</v>
+        <f t="shared" si="8"/>
+        <v>90</v>
       </c>
       <c r="F47" s="5" t="s">
         <v>127</v>
@@ -3609,10 +3647,10 @@
       </c>
       <c r="H47" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>landandwater_distro[45] = {createworldcode = 43, text = "0",x =1155,y = 75}</v>
+        <v>landandwaterdistro[45] = {createworldcode = 43, text = "0",x =1155,y = 90}</v>
       </c>
       <c r="L47" s="4" t="s">
-        <v>357</v>
+        <v>318</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
@@ -3629,8 +3667,8 @@
         <v>1155</v>
       </c>
       <c r="E48" s="4">
-        <f t="shared" si="7"/>
-        <v>90</v>
+        <f t="shared" si="8"/>
+        <v>105</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>127</v>
@@ -3641,7 +3679,7 @@
       </c>
       <c r="H48" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>landandwater_distro[46] = {createworldcode = 44, text = "0",x =1155,y = 90}</v>
+        <v>landandwaterdistro[46] = {createworldcode = 44, text = "0",x =1155,y = 105}</v>
       </c>
       <c r="L48" s="4" t="s">
         <v>358</v>
@@ -3661,8 +3699,8 @@
         <v>1155</v>
       </c>
       <c r="E49" s="4">
-        <f t="shared" si="7"/>
-        <v>105</v>
+        <f t="shared" si="8"/>
+        <v>120</v>
       </c>
       <c r="F49" s="5" t="s">
         <v>127</v>
@@ -3673,7 +3711,7 @@
       </c>
       <c r="H49" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>landandwater_distro[47] = {createworldcode = 45, text = "0",x =1155,y = 105}</v>
+        <v>landandwaterdistro[47] = {createworldcode = 45, text = "0",x =1155,y = 120}</v>
       </c>
       <c r="L49" s="4" t="s">
         <v>359</v>
@@ -3693,8 +3731,8 @@
         <v>1155</v>
       </c>
       <c r="E50" s="4">
-        <f t="shared" si="7"/>
-        <v>120</v>
+        <f t="shared" si="8"/>
+        <v>135</v>
       </c>
       <c r="F50" s="5" t="s">
         <v>127</v>
@@ -3705,7 +3743,7 @@
       </c>
       <c r="H50" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>landandwater_distro[48] = {createworldcode = 46, text = "0",x =1155,y = 120}</v>
+        <v>landandwaterdistro[48] = {createworldcode = 46, text = "0",x =1155,y = 135}</v>
       </c>
       <c r="L50" s="4" t="s">
         <v>360</v>
@@ -3725,8 +3763,8 @@
         <v>1155</v>
       </c>
       <c r="E51" s="4">
-        <f t="shared" si="7"/>
-        <v>135</v>
+        <f t="shared" si="8"/>
+        <v>150</v>
       </c>
       <c r="F51" s="5" t="s">
         <v>127</v>
@@ -3737,7 +3775,7 @@
       </c>
       <c r="H51" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>landandwater_distro[49] = {createworldcode = 47, text = "0",x =1155,y = 135}</v>
+        <v>landandwaterdistro[49] = {createworldcode = 47, text = "0",x =1155,y = 150}</v>
       </c>
       <c r="L51" s="4" t="s">
         <v>361</v>
@@ -3753,112 +3791,102 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5703125" customWidth="1"/>
     <col min="3" max="5" width="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>308</v>
+      </c>
+    </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="8">
+      <c r="A2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="8">
         <v>20</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C3" s="8">
         <v>40</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D3" s="8">
         <v>60</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E3" s="8">
         <v>80</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F3" s="8">
         <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>301</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>8</v>
-      </c>
-      <c r="F3">
-        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E4">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F4">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
         <v>4</v>
       </c>
-      <c r="D5">
-        <v>5</v>
-      </c>
       <c r="E5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <v>4</v>
       </c>
       <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
         <v>4</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -3866,19 +3894,19 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -3886,16 +3914,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C8">
         <v>3</v>
       </c>
       <c r="D8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -3906,21 +3934,41 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C9">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>307</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
         <v>0</v>
       </c>
     </row>
@@ -5102,574 +5150,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O29" sqref="O29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D1" t="s">
-        <v>136</v>
-      </c>
-      <c r="F1" t="s">
-        <v>137</v>
-      </c>
-      <c r="J1" t="s">
-        <v>135</v>
-      </c>
-      <c r="K1" t="s">
-        <v>136</v>
-      </c>
-      <c r="L1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>138</v>
-      </c>
-      <c r="C2" t="s">
-        <v>139</v>
-      </c>
-      <c r="D2" t="s">
-        <v>138</v>
-      </c>
-      <c r="E2" t="s">
-        <v>139</v>
-      </c>
-      <c r="F2" t="s">
-        <v>138</v>
-      </c>
-      <c r="G2" t="s">
-        <v>139</v>
-      </c>
-      <c r="J2" t="s">
-        <v>208</v>
-      </c>
-      <c r="K2" t="s">
-        <v>208</v>
-      </c>
-      <c r="L2" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>800</v>
-      </c>
-      <c r="C3">
-        <v>1287.4752000000001</v>
-      </c>
-      <c r="D3">
-        <v>50</v>
-      </c>
-      <c r="E3">
-        <v>80.467200000000005</v>
-      </c>
-      <c r="F3">
-        <v>10</v>
-      </c>
-      <c r="G3">
-        <v>16.093440000000001</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3" t="str">
-        <f>CONCATENATE(C3," ( ",B3," )")</f>
-        <v>1287.4752 ( 800 )</v>
-      </c>
-      <c r="K3" t="str">
-        <f>CONCATENATE(E3," ( ",D3," )")</f>
-        <v>80.4672 ( 50 )</v>
-      </c>
-      <c r="L3" t="str">
-        <f>CONCATENATE(G3," ( ",F3," )")</f>
-        <v>16.09344 ( 10 )</v>
-      </c>
-      <c r="N3" t="e">
-        <f>conc</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>1600</v>
-      </c>
-      <c r="C4">
-        <v>2574.9504000000002</v>
-      </c>
-      <c r="D4">
-        <v>100</v>
-      </c>
-      <c r="E4">
-        <v>160.93440000000001</v>
-      </c>
-      <c r="F4">
-        <v>20</v>
-      </c>
-      <c r="G4">
-        <v>32.186880000000002</v>
-      </c>
-      <c r="I4">
-        <v>2</v>
-      </c>
-      <c r="J4" t="str">
-        <f t="shared" ref="J4:J11" si="0">CONCATENATE(C4," ( ",B4," )")</f>
-        <v>2574.9504 ( 1600 )</v>
-      </c>
-      <c r="K4" t="str">
-        <f t="shared" ref="K4:K11" si="1">CONCATENATE(E4," ( ",D4," )")</f>
-        <v>160.9344 ( 100 )</v>
-      </c>
-      <c r="L4" t="str">
-        <f t="shared" ref="L4:L11" si="2">CONCATENATE(G4," ( ",F4," )")</f>
-        <v>32.18688 ( 20 )</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>2400</v>
-      </c>
-      <c r="C5">
-        <v>3862.4256000000005</v>
-      </c>
-      <c r="D5">
-        <v>150</v>
-      </c>
-      <c r="E5">
-        <v>241.40160000000003</v>
-      </c>
-      <c r="F5">
-        <v>30</v>
-      </c>
-      <c r="G5">
-        <v>48.280320000000003</v>
-      </c>
-      <c r="I5">
-        <v>3</v>
-      </c>
-      <c r="J5" t="str">
-        <f t="shared" si="0"/>
-        <v>3862.4256 ( 2400 )</v>
-      </c>
-      <c r="K5" t="str">
-        <f t="shared" si="1"/>
-        <v>241.4016 ( 150 )</v>
-      </c>
-      <c r="L5" t="str">
-        <f t="shared" si="2"/>
-        <v>48.28032 ( 30 )</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>4000</v>
-      </c>
-      <c r="C6">
-        <v>6437.3760000000002</v>
-      </c>
-      <c r="D6">
-        <v>250</v>
-      </c>
-      <c r="E6">
-        <v>402.33600000000001</v>
-      </c>
-      <c r="F6">
-        <v>50</v>
-      </c>
-      <c r="G6">
-        <v>80.467200000000005</v>
-      </c>
-      <c r="I6">
-        <v>4</v>
-      </c>
-      <c r="J6" t="str">
-        <f t="shared" si="0"/>
-        <v>6437.376 ( 4000 )</v>
-      </c>
-      <c r="K6" t="str">
-        <f t="shared" si="1"/>
-        <v>402.336 ( 250 )</v>
-      </c>
-      <c r="L6" t="str">
-        <f t="shared" si="2"/>
-        <v>80.4672 ( 50 )</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>4800</v>
-      </c>
-      <c r="C7">
-        <v>7724.851200000001</v>
-      </c>
-      <c r="D7">
-        <v>300</v>
-      </c>
-      <c r="E7">
-        <v>482.80320000000006</v>
-      </c>
-      <c r="F7">
-        <v>60</v>
-      </c>
-      <c r="G7">
-        <v>96.560640000000006</v>
-      </c>
-      <c r="I7">
-        <v>5</v>
-      </c>
-      <c r="J7" t="str">
-        <f t="shared" si="0"/>
-        <v>7724.8512 ( 4800 )</v>
-      </c>
-      <c r="K7" t="str">
-        <f t="shared" si="1"/>
-        <v>482.8032 ( 300 )</v>
-      </c>
-      <c r="L7" t="str">
-        <f t="shared" si="2"/>
-        <v>96.56064 ( 60 )</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>8000</v>
-      </c>
-      <c r="C8">
-        <v>12874.752</v>
-      </c>
-      <c r="D8">
-        <v>500</v>
-      </c>
-      <c r="E8">
-        <v>804.67200000000003</v>
-      </c>
-      <c r="F8">
-        <v>100</v>
-      </c>
-      <c r="G8">
-        <v>160.93440000000001</v>
-      </c>
-      <c r="I8">
-        <v>6</v>
-      </c>
-      <c r="J8" t="str">
-        <f t="shared" si="0"/>
-        <v>12874.752 ( 8000 )</v>
-      </c>
-      <c r="K8" t="str">
-        <f t="shared" si="1"/>
-        <v>804.672 ( 500 )</v>
-      </c>
-      <c r="L8" t="str">
-        <f t="shared" si="2"/>
-        <v>160.9344 ( 100 )</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>10000</v>
-      </c>
-      <c r="C9">
-        <v>16093.44</v>
-      </c>
-      <c r="D9">
-        <v>625</v>
-      </c>
-      <c r="E9">
-        <v>1005.84</v>
-      </c>
-      <c r="F9">
-        <v>125</v>
-      </c>
-      <c r="G9">
-        <v>201.16800000000001</v>
-      </c>
-      <c r="I9">
-        <v>7</v>
-      </c>
-      <c r="J9" t="str">
-        <f t="shared" si="0"/>
-        <v>16093.44 ( 10000 )</v>
-      </c>
-      <c r="K9" t="str">
-        <f t="shared" si="1"/>
-        <v>1005.84 ( 625 )</v>
-      </c>
-      <c r="L9" t="str">
-        <f t="shared" si="2"/>
-        <v>201.168 ( 125 )</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>12000</v>
-      </c>
-      <c r="C10">
-        <v>19312.128000000001</v>
-      </c>
-      <c r="D10">
-        <v>750</v>
-      </c>
-      <c r="E10">
-        <v>1207.008</v>
-      </c>
-      <c r="F10">
-        <v>150</v>
-      </c>
-      <c r="G10">
-        <v>241.40160000000003</v>
-      </c>
-      <c r="I10">
-        <v>8</v>
-      </c>
-      <c r="J10" t="str">
-        <f t="shared" si="0"/>
-        <v>19312.128 ( 12000 )</v>
-      </c>
-      <c r="K10" t="str">
-        <f t="shared" si="1"/>
-        <v>1207.008 ( 750 )</v>
-      </c>
-      <c r="L10" t="str">
-        <f t="shared" si="2"/>
-        <v>241.4016 ( 150 )</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <v>16000</v>
-      </c>
-      <c r="C11">
-        <v>25749.504000000001</v>
-      </c>
-      <c r="D11">
-        <v>1000</v>
-      </c>
-      <c r="E11">
-        <v>1609.3440000000001</v>
-      </c>
-      <c r="F11">
-        <v>200</v>
-      </c>
-      <c r="G11">
-        <v>321.86880000000002</v>
-      </c>
-      <c r="I11">
-        <v>9</v>
-      </c>
-      <c r="J11" t="str">
-        <f t="shared" si="0"/>
-        <v>25749.504 ( 16000 )</v>
-      </c>
-      <c r="K11" t="str">
-        <f t="shared" si="1"/>
-        <v>1609.344 ( 1000 )</v>
-      </c>
-      <c r="L11" t="str">
-        <f t="shared" si="2"/>
-        <v>321.8688 ( 200 )</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J13" t="s">
-        <v>135</v>
-      </c>
-      <c r="K13" t="s">
-        <v>136</v>
-      </c>
-      <c r="L13" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J14" t="s">
-        <v>208</v>
-      </c>
-      <c r="K14" t="s">
-        <v>208</v>
-      </c>
-      <c r="L14" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I15">
-        <v>1</v>
-      </c>
-      <c r="J15" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="K15" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="L15" s="7" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I16">
-        <v>2</v>
-      </c>
-      <c r="J16" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="K16" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="L16" s="7" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="17" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I17">
-        <v>3</v>
-      </c>
-      <c r="J17" s="7" t="s">
-        <v>215</v>
-      </c>
-      <c r="K17" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="L17" s="7" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="18" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I18">
-        <v>4</v>
-      </c>
-      <c r="J18" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="K18" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="L18" s="7" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="19" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I19">
-        <v>5</v>
-      </c>
-      <c r="J19" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="K19" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="L19" s="7" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="20" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I20">
-        <v>6</v>
-      </c>
-      <c r="J20" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="K20" s="7" t="s">
-        <v>224</v>
-      </c>
-      <c r="L20" s="7" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="21" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I21">
-        <v>7</v>
-      </c>
-      <c r="J21" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="K21" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="L21" s="7" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="22" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I22">
-        <v>8</v>
-      </c>
-      <c r="J22" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="K22" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="L22" s="7" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="23" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I23">
-        <v>9</v>
-      </c>
-      <c r="J23" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="K23" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="L23" s="7" t="s">
-        <v>232</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N72"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="bottomLeft" activeCell="G60" sqref="G60"/>
     </sheetView>
@@ -5728,11 +5212,11 @@
         <v>127</v>
       </c>
       <c r="E3" s="2" t="str">
-        <f>CONCATENATE(D3,C3,D3)</f>
+        <f t="shared" ref="E3:E34" si="0">CONCATENATE(D3,C3,D3)</f>
         <v>"--[[[Cultural Climate or landform]]]--"</v>
       </c>
       <c r="F3" s="1" t="str">
-        <f>CONCATENATE($C$1,A3," = ","{",$B$2," = ",B3,", ",$C$2," = ",E3,",",$G$2,G3,",",$H$2,H3,"}","")</f>
+        <f t="shared" ref="F3:F34" si="1">CONCATENATE($C$1,A3," = ","{",$B$2," = ",B3,", ",$C$2," = ",E3,",",$G$2,G3,",",$H$2,H3,"}","")</f>
         <v>worldhooks[1] = {createworldcode = 0, text = "--[[[Cultural Climate or landform]]]--",x =755,y = 30}</v>
       </c>
       <c r="G3" s="1">
@@ -5759,11 +5243,11 @@
         <v>127</v>
       </c>
       <c r="E4" s="2" t="str">
-        <f>CONCATENATE(D4,C4,D4)</f>
+        <f t="shared" si="0"/>
         <v>"--[[[Cultural Situation]]]--"</v>
       </c>
       <c r="F4" s="1" t="str">
-        <f>CONCATENATE($C$1,A4," = ","{",$B$2," = ",B4,", ",$C$2," = ",E4,",",$G$2,G4,",",$H$2,H4,"}","")</f>
+        <f t="shared" si="1"/>
         <v>worldhooks[40] = {createworldcode = 0, text = "--[[[Cultural Situation]]]--",x =755,y = 75}</v>
       </c>
       <c r="G4" s="1">
@@ -5791,11 +5275,11 @@
         <v>127</v>
       </c>
       <c r="E5" s="2" t="str">
-        <f>CONCATENATE(D5,C5,D5)</f>
+        <f t="shared" si="0"/>
         <v>"--[[[Cultural Sites of Interest]]]--"</v>
       </c>
       <c r="F5" s="1" t="str">
-        <f>CONCATENATE($C$1,A5," = ","{",$B$2," = ",B5,", ",$C$2," = ",E5,",",$G$2,G5,",",$H$2,H5,"}","")</f>
+        <f t="shared" si="1"/>
         <v>worldhooks[18] = {createworldcode = 0, text = "--[[[Cultural Sites of Interest]]]--",x =1055,y = 30}</v>
       </c>
       <c r="G5" s="3">
@@ -5822,11 +5306,11 @@
         <v>127</v>
       </c>
       <c r="E6" s="2" t="str">
-        <f>CONCATENATE(D6,C6,D6)</f>
+        <f t="shared" si="0"/>
         <v>"--[[[Cultural Theme]]]--"</v>
       </c>
       <c r="F6" s="1" t="str">
-        <f>CONCATENATE($C$1,A6," = ","{",$B$2," = ",B6,", ",$C$2," = ",E6,",",$G$2,G6,",",$H$2,H6,"}","")</f>
+        <f t="shared" si="1"/>
         <v>worldhooks[27] = {createworldcode = 0, text = "--[[[Cultural Theme]]]--",x =1055,y = 75}</v>
       </c>
       <c r="G6" s="3">
@@ -5854,11 +5338,11 @@
         <v>127</v>
       </c>
       <c r="E7" s="2" t="str">
-        <f>CONCATENATE(D7,C7,D7)</f>
+        <f t="shared" si="0"/>
         <v>"--[[[Cultural History]]]--"</v>
       </c>
       <c r="F7" s="1" t="str">
-        <f>CONCATENATE($C$1,A7," = ","{",$B$2," = ",B7,", ",$C$2," = ",E7,",",$G$2,G7,",",$H$2,H7,"}","")</f>
+        <f t="shared" si="1"/>
         <v>worldhooks[57] = {createworldcode = 0, text = "--[[[Cultural History]]]--",x =1055,y = 120}</v>
       </c>
       <c r="G7" s="1">
@@ -5886,18 +5370,18 @@
         <v>127</v>
       </c>
       <c r="E8" s="2" t="str">
-        <f>CONCATENATE(D8,C8,D8)</f>
+        <f t="shared" si="0"/>
         <v>"Aerial"</v>
       </c>
       <c r="F8" s="1" t="str">
-        <f>CONCATENATE($C$1,A8," = ","{",$B$2," = ",B8,", ",$C$2," = ",E8,",",$G$2,G8,",",$H$2,H8,"}","")</f>
+        <f t="shared" si="1"/>
         <v>worldhooks[2] = {createworldcode = 1, text = "Aerial",x =755,y = 135}</v>
       </c>
       <c r="G8" s="1">
         <v>755</v>
       </c>
       <c r="H8" s="1">
-        <f>H7+$N$1</f>
+        <f t="shared" ref="H8:H23" si="2">H7+$N$1</f>
         <v>135</v>
       </c>
       <c r="L8" s="1" t="s">
@@ -5918,18 +5402,18 @@
         <v>127</v>
       </c>
       <c r="E9" s="2" t="str">
-        <f>CONCATENATE(D9,C9,D9)</f>
+        <f t="shared" si="0"/>
         <v>"Archipelago"</v>
       </c>
       <c r="F9" s="1" t="str">
-        <f>CONCATENATE($C$1,A9," = ","{",$B$2," = ",B9,", ",$C$2," = ",E9,",",$G$2,G9,",",$H$2,H9,"}","")</f>
+        <f t="shared" si="1"/>
         <v>worldhooks[3] = {createworldcode = 2, text = "Archipelago",x =755,y = 150}</v>
       </c>
       <c r="G9" s="1">
         <v>755</v>
       </c>
       <c r="H9" s="1">
-        <f>H8+$N$1</f>
+        <f t="shared" si="2"/>
         <v>150</v>
       </c>
       <c r="L9" s="1" t="s">
@@ -5950,18 +5434,18 @@
         <v>127</v>
       </c>
       <c r="E10" s="2" t="str">
-        <f>CONCATENATE(D10,C10,D10)</f>
+        <f t="shared" si="0"/>
         <v>"Arctic"</v>
       </c>
       <c r="F10" s="1" t="str">
-        <f>CONCATENATE($C$1,A10," = ","{",$B$2," = ",B10,", ",$C$2," = ",E10,",",$G$2,G10,",",$H$2,H10,"}","")</f>
+        <f t="shared" si="1"/>
         <v>worldhooks[4] = {createworldcode = 3, text = "Arctic",x =755,y = 165}</v>
       </c>
       <c r="G10" s="1">
         <v>755</v>
       </c>
       <c r="H10" s="1">
-        <f>H9+$N$1</f>
+        <f t="shared" si="2"/>
         <v>165</v>
       </c>
       <c r="L10" s="1" t="s">
@@ -5982,18 +5466,18 @@
         <v>127</v>
       </c>
       <c r="E11" s="2" t="str">
-        <f>CONCATENATE(D11,C11,D11)</f>
+        <f t="shared" si="0"/>
         <v>"Desert"</v>
       </c>
       <c r="F11" s="1" t="str">
-        <f>CONCATENATE($C$1,A11," = ","{",$B$2," = ",B11,", ",$C$2," = ",E11,",",$G$2,G11,",",$H$2,H11,"}","")</f>
+        <f t="shared" si="1"/>
         <v>worldhooks[5] = {createworldcode = 4, text = "Desert",x =755,y = 180}</v>
       </c>
       <c r="G11" s="1">
         <v>755</v>
       </c>
       <c r="H11" s="1">
-        <f>H10+$N$1</f>
+        <f t="shared" si="2"/>
         <v>180</v>
       </c>
       <c r="L11" s="1" t="s">
@@ -6014,18 +5498,18 @@
         <v>127</v>
       </c>
       <c r="E12" s="2" t="str">
-        <f>CONCATENATE(D12,C12,D12)</f>
+        <f t="shared" si="0"/>
         <v>"Forest"</v>
       </c>
       <c r="F12" s="1" t="str">
-        <f>CONCATENATE($C$1,A12," = ","{",$B$2," = ",B12,", ",$C$2," = ",E12,",",$G$2,G12,",",$H$2,H12,"}","")</f>
+        <f t="shared" si="1"/>
         <v>worldhooks[6] = {createworldcode = 5, text = "Forest",x =755,y = 195}</v>
       </c>
       <c r="G12" s="1">
         <v>755</v>
       </c>
       <c r="H12" s="1">
-        <f>H11+$N$1</f>
+        <f t="shared" si="2"/>
         <v>195</v>
       </c>
       <c r="L12" s="1" t="s">
@@ -6046,18 +5530,18 @@
         <v>127</v>
       </c>
       <c r="E13" s="2" t="str">
-        <f>CONCATENATE(D13,C13,D13)</f>
+        <f t="shared" si="0"/>
         <v>"Inland Sea / lake"</v>
       </c>
       <c r="F13" s="1" t="str">
-        <f>CONCATENATE($C$1,A13," = ","{",$B$2," = ",B13,", ",$C$2," = ",E13,",",$G$2,G13,",",$H$2,H13,"}","")</f>
+        <f t="shared" si="1"/>
         <v>worldhooks[7] = {createworldcode = 6, text = "Inland Sea / lake",x =755,y = 210}</v>
       </c>
       <c r="G13" s="1">
         <v>755</v>
       </c>
       <c r="H13" s="1">
-        <f>H12+$N$1</f>
+        <f t="shared" si="2"/>
         <v>210</v>
       </c>
       <c r="L13" s="1" t="s">
@@ -6078,18 +5562,18 @@
         <v>127</v>
       </c>
       <c r="E14" s="2" t="str">
-        <f>CONCATENATE(D14,C14,D14)</f>
+        <f t="shared" si="0"/>
         <v>"Jungle"</v>
       </c>
       <c r="F14" s="1" t="str">
-        <f>CONCATENATE($C$1,A14," = ","{",$B$2," = ",B14,", ",$C$2," = ",E14,",",$G$2,G14,",",$H$2,H14,"}","")</f>
+        <f t="shared" si="1"/>
         <v>worldhooks[8] = {createworldcode = 7, text = "Jungle",x =755,y = 225}</v>
       </c>
       <c r="G14" s="1">
         <v>755</v>
       </c>
       <c r="H14" s="1">
-        <f>H13+$N$1</f>
+        <f t="shared" si="2"/>
         <v>225</v>
       </c>
       <c r="L14" s="1" t="s">
@@ -6110,18 +5594,18 @@
         <v>127</v>
       </c>
       <c r="E15" s="2" t="str">
-        <f>CONCATENATE(D15,C15,D15)</f>
+        <f t="shared" si="0"/>
         <v>"Mountain "</v>
       </c>
       <c r="F15" s="1" t="str">
-        <f>CONCATENATE($C$1,A15," = ","{",$B$2," = ",B15,", ",$C$2," = ",E15,",",$G$2,G15,",",$H$2,H15,"}","")</f>
+        <f t="shared" si="1"/>
         <v>worldhooks[9] = {createworldcode = 8, text = "Mountain ",x =755,y = 240}</v>
       </c>
       <c r="G15" s="1">
         <v>755</v>
       </c>
       <c r="H15" s="1">
-        <f>H14+$N$1</f>
+        <f t="shared" si="2"/>
         <v>240</v>
       </c>
       <c r="L15" s="1" t="s">
@@ -6142,18 +5626,18 @@
         <v>127</v>
       </c>
       <c r="E16" s="2" t="str">
-        <f>CONCATENATE(D16,C16,D16)</f>
+        <f t="shared" si="0"/>
         <v>"Oceananic"</v>
       </c>
       <c r="F16" s="1" t="str">
-        <f>CONCATENATE($C$1,A16," = ","{",$B$2," = ",B16,", ",$C$2," = ",E16,",",$G$2,G16,",",$H$2,H16,"}","")</f>
+        <f t="shared" si="1"/>
         <v>worldhooks[10] = {createworldcode = 9, text = "Oceananic",x =755,y = 255}</v>
       </c>
       <c r="G16" s="1">
         <v>755</v>
       </c>
       <c r="H16" s="1">
-        <f>H15+$N$1</f>
+        <f t="shared" si="2"/>
         <v>255</v>
       </c>
       <c r="L16" s="1" t="s">
@@ -6174,18 +5658,18 @@
         <v>127</v>
       </c>
       <c r="E17" s="2" t="str">
-        <f>CONCATENATE(D17,C17,D17)</f>
+        <f t="shared" si="0"/>
         <v>"Plains / steppes"</v>
       </c>
       <c r="F17" s="1" t="str">
-        <f>CONCATENATE($C$1,A17," = ","{",$B$2," = ",B17,", ",$C$2," = ",E17,",",$G$2,G17,",",$H$2,H17,"}","")</f>
+        <f t="shared" si="1"/>
         <v>worldhooks[11] = {createworldcode = 10, text = "Plains / steppes",x =755,y = 270}</v>
       </c>
       <c r="G17" s="1">
         <v>755</v>
       </c>
       <c r="H17" s="1">
-        <f>H16+$N$1</f>
+        <f t="shared" si="2"/>
         <v>270</v>
       </c>
       <c r="L17" s="1" t="s">
@@ -6206,18 +5690,18 @@
         <v>127</v>
       </c>
       <c r="E18" s="2" t="str">
-        <f>CONCATENATE(D18,C18,D18)</f>
+        <f t="shared" si="0"/>
         <v>"Subterranean"</v>
       </c>
       <c r="F18" s="1" t="str">
-        <f>CONCATENATE($C$1,A18," = ","{",$B$2," = ",B18,", ",$C$2," = ",E18,",",$G$2,G18,",",$H$2,H18,"}","")</f>
+        <f t="shared" si="1"/>
         <v>worldhooks[12] = {createworldcode = 11, text = "Subterranean",x =755,y = 285}</v>
       </c>
       <c r="G18" s="1">
         <v>755</v>
       </c>
       <c r="H18" s="1">
-        <f>H17+$N$1</f>
+        <f t="shared" si="2"/>
         <v>285</v>
       </c>
       <c r="L18" s="1" t="s">
@@ -6238,18 +5722,18 @@
         <v>127</v>
       </c>
       <c r="E19" s="2" t="str">
-        <f>CONCATENATE(D19,C19,D19)</f>
+        <f t="shared" si="0"/>
         <v>"Swamp"</v>
       </c>
       <c r="F19" s="1" t="str">
-        <f>CONCATENATE($C$1,A19," = ","{",$B$2," = ",B19,", ",$C$2," = ",E19,",",$G$2,G19,",",$H$2,H19,"}","")</f>
+        <f t="shared" si="1"/>
         <v>worldhooks[13] = {createworldcode = 12, text = "Swamp",x =755,y = 300}</v>
       </c>
       <c r="G19" s="1">
         <v>755</v>
       </c>
       <c r="H19" s="1">
-        <f>H18+$N$1</f>
+        <f t="shared" si="2"/>
         <v>300</v>
       </c>
       <c r="L19" s="1" t="s">
@@ -6270,18 +5754,18 @@
         <v>127</v>
       </c>
       <c r="E20" s="2" t="str">
-        <f>CONCATENATE(D20,C20,D20)</f>
+        <f t="shared" si="0"/>
         <v>"Uninhabitable"</v>
       </c>
       <c r="F20" s="1" t="str">
-        <f>CONCATENATE($C$1,A20," = ","{",$B$2," = ",B20,", ",$C$2," = ",E20,",",$G$2,G20,",",$H$2,H20,"}","")</f>
+        <f t="shared" si="1"/>
         <v>worldhooks[14] = {createworldcode = 13, text = "Uninhabitable",x =755,y = 315}</v>
       </c>
       <c r="G20" s="1">
         <v>755</v>
       </c>
       <c r="H20" s="1">
-        <f>H19+$N$1</f>
+        <f t="shared" si="2"/>
         <v>315</v>
       </c>
       <c r="L20" s="1" t="s">
@@ -6302,18 +5786,18 @@
         <v>127</v>
       </c>
       <c r="E21" s="2" t="str">
-        <f>CONCATENATE(D21,C21,D21)</f>
+        <f t="shared" si="0"/>
         <v>"Unstable / formless"</v>
       </c>
       <c r="F21" s="1" t="str">
-        <f>CONCATENATE($C$1,A21," = ","{",$B$2," = ",B21,", ",$C$2," = ",E21,",",$G$2,G21,",",$H$2,H21,"}","")</f>
+        <f t="shared" si="1"/>
         <v>worldhooks[15] = {createworldcode = 14, text = "Unstable / formless",x =755,y = 330}</v>
       </c>
       <c r="G21" s="1">
         <v>755</v>
       </c>
       <c r="H21" s="1">
-        <f>H20+$N$1</f>
+        <f t="shared" si="2"/>
         <v>330</v>
       </c>
       <c r="L21" s="1" t="s">
@@ -6334,18 +5818,18 @@
         <v>127</v>
       </c>
       <c r="E22" s="2" t="str">
-        <f>CONCATENATE(D22,C22,D22)</f>
+        <f t="shared" si="0"/>
         <v>"Volcanic"</v>
       </c>
       <c r="F22" s="1" t="str">
-        <f>CONCATENATE($C$1,A22," = ","{",$B$2," = ",B22,", ",$C$2," = ",E22,",",$G$2,G22,",",$H$2,H22,"}","")</f>
+        <f t="shared" si="1"/>
         <v>worldhooks[16] = {createworldcode = 15, text = "Volcanic",x =755,y = 345}</v>
       </c>
       <c r="G22" s="1">
         <v>755</v>
       </c>
       <c r="H22" s="1">
-        <f>H21+$N$1</f>
+        <f t="shared" si="2"/>
         <v>345</v>
       </c>
       <c r="L22" s="1" t="s">
@@ -6366,18 +5850,18 @@
         <v>127</v>
       </c>
       <c r="E23" s="2" t="str">
-        <f>CONCATENATE(D23,C23,D23)</f>
+        <f t="shared" si="0"/>
         <v>"Strage/Unique Weather"</v>
       </c>
       <c r="F23" s="1" t="str">
-        <f>CONCATENATE($C$1,A23," = ","{",$B$2," = ",B23,", ",$C$2," = ",E23,",",$G$2,G23,",",$H$2,H23,"}","")</f>
+        <f t="shared" si="1"/>
         <v>worldhooks[17] = {createworldcode = 16, text = "Strage/Unique Weather",x =755,y = 360}</v>
       </c>
       <c r="G23" s="1">
         <v>755</v>
       </c>
       <c r="H23" s="1">
-        <f>H22+$N$1</f>
+        <f t="shared" si="2"/>
         <v>360</v>
       </c>
       <c r="L23" s="1" t="s">
@@ -6398,11 +5882,11 @@
         <v>127</v>
       </c>
       <c r="E24" s="2" t="str">
-        <f>CONCATENATE(D24,C24,D24)</f>
+        <f t="shared" si="0"/>
         <v>"Caverns"</v>
       </c>
       <c r="F24" s="1" t="str">
-        <f>CONCATENATE($C$1,A24," = ","{",$B$2," = ",B24,", ",$C$2," = ",E24,",",$G$2,G24,",",$H$2,H24,"}","")</f>
+        <f t="shared" si="1"/>
         <v>worldhooks[19] = {createworldcode = 17, text = "Caverns",x =1055,y = 42}</v>
       </c>
       <c r="G24" s="3">
@@ -6429,11 +5913,11 @@
         <v>127</v>
       </c>
       <c r="E25" s="2" t="str">
-        <f>CONCATENATE(D25,C25,D25)</f>
+        <f t="shared" si="0"/>
         <v>"Cites"</v>
       </c>
       <c r="F25" s="1" t="str">
-        <f>CONCATENATE($C$1,A25," = ","{",$B$2," = ",B25,", ",$C$2," = ",E25,",",$G$2,G25,",",$H$2,H25,"}","")</f>
+        <f t="shared" si="1"/>
         <v>worldhooks[20] = {createworldcode = 18, text = "Cites",x =1055,y = 54}</v>
       </c>
       <c r="G25" s="3">
@@ -6460,11 +5944,11 @@
         <v>127</v>
       </c>
       <c r="E26" s="2" t="str">
-        <f>CONCATENATE(D26,C26,D26)</f>
+        <f t="shared" si="0"/>
         <v>"Dungeons"</v>
       </c>
       <c r="F26" s="1" t="str">
-        <f>CONCATENATE($C$1,A26," = ","{",$B$2," = ",B26,", ",$C$2," = ",E26,",",$G$2,G26,",",$H$2,H26,"}","")</f>
+        <f t="shared" si="1"/>
         <v>worldhooks[21] = {createworldcode = 19, text = "Dungeons",x =1055,y = 66}</v>
       </c>
       <c r="G26" s="3">
@@ -6491,11 +5975,11 @@
         <v>127</v>
       </c>
       <c r="E27" s="2" t="str">
-        <f>CONCATENATE(D27,C27,D27)</f>
+        <f t="shared" si="0"/>
         <v>"Extraplanar"</v>
       </c>
       <c r="F27" s="1" t="str">
-        <f>CONCATENATE($C$1,A27," = ","{",$B$2," = ",B27,", ",$C$2," = ",E27,",",$G$2,G27,",",$H$2,H27,"}","")</f>
+        <f t="shared" si="1"/>
         <v>worldhooks[22] = {createworldcode = 20, text = "Extraplanar",x =1055,y = 78}</v>
       </c>
       <c r="G27" s="3">
@@ -6522,11 +6006,11 @@
         <v>127</v>
       </c>
       <c r="E28" s="2" t="str">
-        <f>CONCATENATE(D28,C28,D28)</f>
+        <f t="shared" si="0"/>
         <v>"Fortress / strongholds"</v>
       </c>
       <c r="F28" s="1" t="str">
-        <f>CONCATENATE($C$1,A28," = ","{",$B$2," = ",B28,", ",$C$2," = ",E28,",",$G$2,G28,",",$H$2,H28,"}","")</f>
+        <f t="shared" si="1"/>
         <v>worldhooks[23] = {createworldcode = 21, text = "Fortress / strongholds",x =1055,y = 90}</v>
       </c>
       <c r="G28" s="3">
@@ -6553,11 +6037,11 @@
         <v>127</v>
       </c>
       <c r="E29" s="2" t="str">
-        <f>CONCATENATE(D29,C29,D29)</f>
+        <f t="shared" si="0"/>
         <v>"Ruins"</v>
       </c>
       <c r="F29" s="1" t="str">
-        <f>CONCATENATE($C$1,A29," = ","{",$B$2," = ",B29,", ",$C$2," = ",E29,",",$G$2,G29,",",$H$2,H29,"}","")</f>
+        <f t="shared" si="1"/>
         <v>worldhooks[24] = {createworldcode = 22, text = "Ruins",x =1055,y = 102}</v>
       </c>
       <c r="G29" s="3">
@@ -6584,11 +6068,11 @@
         <v>127</v>
       </c>
       <c r="E30" s="2" t="str">
-        <f>CONCATENATE(D30,C30,D30)</f>
+        <f t="shared" si="0"/>
         <v>"Shrines"</v>
       </c>
       <c r="F30" s="1" t="str">
-        <f>CONCATENATE($C$1,A30," = ","{",$B$2," = ",B30,", ",$C$2," = ",E30,",",$G$2,G30,",",$H$2,H30,"}","")</f>
+        <f t="shared" si="1"/>
         <v>worldhooks[25] = {createworldcode = 23, text = "Shrines",x =1055,y = 114}</v>
       </c>
       <c r="G30" s="3">
@@ -6615,11 +6099,11 @@
         <v>127</v>
       </c>
       <c r="E31" s="2" t="str">
-        <f>CONCATENATE(D31,C31,D31)</f>
+        <f t="shared" si="0"/>
         <v>"Wilderness"</v>
       </c>
       <c r="F31" s="1" t="str">
-        <f>CONCATENATE($C$1,A31," = ","{",$B$2," = ",B31,", ",$C$2," = ",E31,",",$G$2,G31,",",$H$2,H31,"}","")</f>
+        <f t="shared" si="1"/>
         <v>worldhooks[26] = {createworldcode = 24, text = "Wilderness",x =1055,y = 126}</v>
       </c>
       <c r="G31" s="3">
@@ -6646,18 +6130,18 @@
         <v>127</v>
       </c>
       <c r="E32" s="2" t="str">
-        <f>CONCATENATE(D32,C32,D32)</f>
+        <f t="shared" si="0"/>
         <v>"African"</v>
       </c>
       <c r="F32" s="1" t="str">
-        <f>CONCATENATE($C$1,A32," = ","{",$B$2," = ",B32,", ",$C$2," = ",E32,",",$G$2,G32,",",$H$2,H32,"}","")</f>
+        <f t="shared" si="1"/>
         <v>worldhooks[28] = {createworldcode = 25, text = "African",x =1055,y = 141}</v>
       </c>
       <c r="G32" s="3">
         <v>1055</v>
       </c>
       <c r="H32" s="1">
-        <f>H31+$N$1</f>
+        <f t="shared" ref="H32:H67" si="3">H31+$N$1</f>
         <v>141</v>
       </c>
       <c r="L32" s="1" t="s">
@@ -6678,18 +6162,18 @@
         <v>127</v>
       </c>
       <c r="E33" s="2" t="str">
-        <f>CONCATENATE(D33,C33,D33)</f>
+        <f t="shared" si="0"/>
         <v>"Ancient"</v>
       </c>
       <c r="F33" s="1" t="str">
-        <f>CONCATENATE($C$1,A33," = ","{",$B$2," = ",B33,", ",$C$2," = ",E33,",",$G$2,G33,",",$H$2,H33,"}","")</f>
+        <f t="shared" si="1"/>
         <v>worldhooks[29] = {createworldcode = 26, text = "Ancient",x =1055,y = 156}</v>
       </c>
       <c r="G33" s="3">
         <v>1055</v>
       </c>
       <c r="H33" s="1">
-        <f>H32+$N$1</f>
+        <f t="shared" si="3"/>
         <v>156</v>
       </c>
       <c r="L33" s="1" t="s">
@@ -6710,18 +6194,18 @@
         <v>127</v>
       </c>
       <c r="E34" s="2" t="str">
-        <f>CONCATENATE(D34,C34,D34)</f>
+        <f t="shared" si="0"/>
         <v>"Arabian"</v>
       </c>
       <c r="F34" s="1" t="str">
-        <f>CONCATENATE($C$1,A34," = ","{",$B$2," = ",B34,", ",$C$2," = ",E34,",",$G$2,G34,",",$H$2,H34,"}","")</f>
+        <f t="shared" si="1"/>
         <v>worldhooks[30] = {createworldcode = 27, text = "Arabian",x =1055,y = 171}</v>
       </c>
       <c r="G34" s="3">
         <v>1055</v>
       </c>
       <c r="H34" s="1">
-        <f>H33+$N$1</f>
+        <f t="shared" si="3"/>
         <v>171</v>
       </c>
       <c r="L34" s="1" t="s">
@@ -6742,18 +6226,18 @@
         <v>127</v>
       </c>
       <c r="E35" s="2" t="str">
-        <f>CONCATENATE(D35,C35,D35)</f>
+        <f t="shared" ref="E35:E66" si="4">CONCATENATE(D35,C35,D35)</f>
         <v>"Barbarian"</v>
       </c>
       <c r="F35" s="1" t="str">
-        <f>CONCATENATE($C$1,A35," = ","{",$B$2," = ",B35,", ",$C$2," = ",E35,",",$G$2,G35,",",$H$2,H35,"}","")</f>
+        <f t="shared" ref="F35:F66" si="5">CONCATENATE($C$1,A35," = ","{",$B$2," = ",B35,", ",$C$2," = ",E35,",",$G$2,G35,",",$H$2,H35,"}","")</f>
         <v>worldhooks[31] = {createworldcode = 28, text = "Barbarian",x =1055,y = 186}</v>
       </c>
       <c r="G35" s="3">
         <v>1055</v>
       </c>
       <c r="H35" s="1">
-        <f>H34+$N$1</f>
+        <f t="shared" si="3"/>
         <v>186</v>
       </c>
       <c r="L35" s="1" t="s">
@@ -6774,18 +6258,18 @@
         <v>127</v>
       </c>
       <c r="E36" s="2" t="str">
-        <f>CONCATENATE(D36,C36,D36)</f>
+        <f t="shared" si="4"/>
         <v>"Feudal"</v>
       </c>
       <c r="F36" s="1" t="str">
-        <f>CONCATENATE($C$1,A36," = ","{",$B$2," = ",B36,", ",$C$2," = ",E36,",",$G$2,G36,",",$H$2,H36,"}","")</f>
+        <f t="shared" si="5"/>
         <v>worldhooks[32] = {createworldcode = 29, text = "Feudal",x =1055,y = 201}</v>
       </c>
       <c r="G36" s="3">
         <v>1055</v>
       </c>
       <c r="H36" s="1">
-        <f>H35+$N$1</f>
+        <f t="shared" si="3"/>
         <v>201</v>
       </c>
       <c r="L36" s="1" t="s">
@@ -6806,18 +6290,18 @@
         <v>127</v>
       </c>
       <c r="E37" s="2" t="str">
-        <f>CONCATENATE(D37,C37,D37)</f>
+        <f t="shared" si="4"/>
         <v>"Mercantile"</v>
       </c>
       <c r="F37" s="1" t="str">
-        <f>CONCATENATE($C$1,A37," = ","{",$B$2," = ",B37,", ",$C$2," = ",E37,",",$G$2,G37,",",$H$2,H37,"}","")</f>
+        <f t="shared" si="5"/>
         <v>worldhooks[33] = {createworldcode = 30, text = "Mercantile",x =1055,y = 216}</v>
       </c>
       <c r="G37" s="3">
         <v>1055</v>
       </c>
       <c r="H37" s="1">
-        <f>H36+$N$1</f>
+        <f t="shared" si="3"/>
         <v>216</v>
       </c>
       <c r="L37" s="1" t="s">
@@ -6838,18 +6322,18 @@
         <v>127</v>
       </c>
       <c r="E38" s="2" t="str">
-        <f>CONCATENATE(D38,C38,D38)</f>
+        <f t="shared" si="4"/>
         <v>"Native American"</v>
       </c>
       <c r="F38" s="1" t="str">
-        <f>CONCATENATE($C$1,A38," = ","{",$B$2," = ",B38,", ",$C$2," = ",E38,",",$G$2,G38,",",$H$2,H38,"}","")</f>
+        <f t="shared" si="5"/>
         <v>worldhooks[34] = {createworldcode = 31, text = "Native American",x =1055,y = 231}</v>
       </c>
       <c r="G38" s="3">
         <v>1055</v>
       </c>
       <c r="H38" s="1">
-        <f>H37+$N$1</f>
+        <f t="shared" si="3"/>
         <v>231</v>
       </c>
       <c r="L38" s="1" t="s">
@@ -6870,18 +6354,18 @@
         <v>127</v>
       </c>
       <c r="E39" s="2" t="str">
-        <f>CONCATENATE(D39,C39,D39)</f>
+        <f t="shared" si="4"/>
         <v>"Oriental"</v>
       </c>
       <c r="F39" s="1" t="str">
-        <f>CONCATENATE($C$1,A39," = ","{",$B$2," = ",B39,", ",$C$2," = ",E39,",",$G$2,G39,",",$H$2,H39,"}","")</f>
+        <f t="shared" si="5"/>
         <v>worldhooks[35] = {createworldcode = 32, text = "Oriental",x =1055,y = 246}</v>
       </c>
       <c r="G39" s="3">
         <v>1055</v>
       </c>
       <c r="H39" s="1">
-        <f>H38+$N$1</f>
+        <f t="shared" si="3"/>
         <v>246</v>
       </c>
       <c r="L39" s="1" t="s">
@@ -6902,18 +6386,18 @@
         <v>127</v>
       </c>
       <c r="E40" s="2" t="str">
-        <f>CONCATENATE(D40,C40,D40)</f>
+        <f t="shared" si="4"/>
         <v>"Renaissance"</v>
       </c>
       <c r="F40" s="1" t="str">
-        <f>CONCATENATE($C$1,A40," = ","{",$B$2," = ",B40,", ",$C$2," = ",E40,",",$G$2,G40,",",$H$2,H40,"}","")</f>
+        <f t="shared" si="5"/>
         <v>worldhooks[36] = {createworldcode = 33, text = "Renaissance",x =1055,y = 261}</v>
       </c>
       <c r="G40" s="3">
         <v>1055</v>
       </c>
       <c r="H40" s="1">
-        <f>H39+$N$1</f>
+        <f t="shared" si="3"/>
         <v>261</v>
       </c>
       <c r="L40" s="1" t="s">
@@ -6934,18 +6418,18 @@
         <v>127</v>
       </c>
       <c r="E41" s="2" t="str">
-        <f>CONCATENATE(D41,C41,D41)</f>
+        <f t="shared" si="4"/>
         <v>"Post Renaissance"</v>
       </c>
       <c r="F41" s="1" t="str">
-        <f>CONCATENATE($C$1,A41," = ","{",$B$2," = ",B41,", ",$C$2," = ",E41,",",$G$2,G41,",",$H$2,H41,"}","")</f>
+        <f t="shared" si="5"/>
         <v>worldhooks[37] = {createworldcode = 34, text = "Post Renaissance",x =1055,y = 276}</v>
       </c>
       <c r="G41" s="3">
         <v>1055</v>
       </c>
       <c r="H41" s="1">
-        <f>H40+$N$1</f>
+        <f t="shared" si="3"/>
         <v>276</v>
       </c>
       <c r="L41" s="1" t="s">
@@ -6966,18 +6450,18 @@
         <v>127</v>
       </c>
       <c r="E42" s="2" t="str">
-        <f>CONCATENATE(D42,C42,D42)</f>
+        <f t="shared" si="4"/>
         <v>"Savage"</v>
       </c>
       <c r="F42" s="1" t="str">
-        <f>CONCATENATE($C$1,A42," = ","{",$B$2," = ",B42,", ",$C$2," = ",E42,",",$G$2,G42,",",$H$2,H42,"}","")</f>
+        <f t="shared" si="5"/>
         <v>worldhooks[38] = {createworldcode = 35, text = "Savage",x =1055,y = 291}</v>
       </c>
       <c r="G42" s="3">
         <v>1055</v>
       </c>
       <c r="H42" s="1">
-        <f>H41+$N$1</f>
+        <f t="shared" si="3"/>
         <v>291</v>
       </c>
       <c r="L42" s="1" t="s">
@@ -6998,18 +6482,18 @@
         <v>127</v>
       </c>
       <c r="E43" s="2" t="str">
-        <f>CONCATENATE(D43,C43,D43)</f>
+        <f t="shared" si="4"/>
         <v>"Seafaring"</v>
       </c>
       <c r="F43" s="1" t="str">
-        <f>CONCATENATE($C$1,A43," = ","{",$B$2," = ",B43,", ",$C$2," = ",E43,",",$G$2,G43,",",$H$2,H43,"}","")</f>
+        <f t="shared" si="5"/>
         <v>worldhooks[39] = {createworldcode = 36, text = "Seafaring",x =1055,y = 306}</v>
       </c>
       <c r="G43" s="3">
         <v>1055</v>
       </c>
       <c r="H43" s="1">
-        <f>H42+$N$1</f>
+        <f t="shared" si="3"/>
         <v>306</v>
       </c>
       <c r="L43" s="1" t="s">
@@ -7030,18 +6514,18 @@
         <v>127</v>
       </c>
       <c r="E44" s="2" t="str">
-        <f>CONCATENATE(D44,C44,D44)</f>
+        <f t="shared" si="4"/>
         <v>"Class Dominance"</v>
       </c>
       <c r="F44" s="1" t="str">
-        <f>CONCATENATE($C$1,A44," = ","{",$B$2," = ",B44,", ",$C$2," = ",E44,",",$G$2,G44,",",$H$2,H44,"}","")</f>
+        <f t="shared" si="5"/>
         <v>worldhooks[41] = {createworldcode = 37, text = "Class Dominance",x =755,y = 321}</v>
       </c>
       <c r="G44" s="1">
         <v>755</v>
       </c>
       <c r="H44" s="1">
-        <f>H43+$N$1</f>
+        <f t="shared" si="3"/>
         <v>321</v>
       </c>
       <c r="L44" s="1" t="s">
@@ -7062,18 +6546,18 @@
         <v>127</v>
       </c>
       <c r="E45" s="2" t="str">
-        <f>CONCATENATE(D45,C45,D45)</f>
+        <f t="shared" si="4"/>
         <v>"Court"</v>
       </c>
       <c r="F45" s="1" t="str">
-        <f>CONCATENATE($C$1,A45," = ","{",$B$2," = ",B45,", ",$C$2," = ",E45,",",$G$2,G45,",",$H$2,H45,"}","")</f>
+        <f t="shared" si="5"/>
         <v>worldhooks[42] = {createworldcode = 38, text = "Court",x =755,y = 336}</v>
       </c>
       <c r="G45" s="1">
         <v>755</v>
       </c>
       <c r="H45" s="1">
-        <f>H44+$N$1</f>
+        <f t="shared" si="3"/>
         <v>336</v>
       </c>
       <c r="L45" s="1" t="s">
@@ -7094,18 +6578,18 @@
         <v>127</v>
       </c>
       <c r="E46" s="2" t="str">
-        <f>CONCATENATE(D46,C46,D46)</f>
+        <f t="shared" si="4"/>
         <v>"Chivalry"</v>
       </c>
       <c r="F46" s="1" t="str">
-        <f>CONCATENATE($C$1,A46," = ","{",$B$2," = ",B46,", ",$C$2," = ",E46,",",$G$2,G46,",",$H$2,H46,"}","")</f>
+        <f t="shared" si="5"/>
         <v>worldhooks[43] = {createworldcode = 39, text = "Chivalry",x =755,y = 351}</v>
       </c>
       <c r="G46" s="1">
         <v>755</v>
       </c>
       <c r="H46" s="1">
-        <f>H45+$N$1</f>
+        <f t="shared" si="3"/>
         <v>351</v>
       </c>
       <c r="L46" s="1" t="s">
@@ -7126,18 +6610,18 @@
         <v>127</v>
       </c>
       <c r="E47" s="2" t="str">
-        <f>CONCATENATE(D47,C47,D47)</f>
+        <f t="shared" si="4"/>
         <v>"Deity"</v>
       </c>
       <c r="F47" s="1" t="str">
-        <f>CONCATENATE($C$1,A47," = ","{",$B$2," = ",B47,", ",$C$2," = ",E47,",",$G$2,G47,",",$H$2,H47,"}","")</f>
+        <f t="shared" si="5"/>
         <v>worldhooks[44] = {createworldcode = 40, text = "Deity",x =755,y = 366}</v>
       </c>
       <c r="G47" s="1">
         <v>755</v>
       </c>
       <c r="H47" s="1">
-        <f>H46+$N$1</f>
+        <f t="shared" si="3"/>
         <v>366</v>
       </c>
       <c r="L47" s="1" t="s">
@@ -7158,18 +6642,18 @@
         <v>127</v>
       </c>
       <c r="E48" s="2" t="str">
-        <f>CONCATENATE(D48,C48,D48)</f>
+        <f t="shared" si="4"/>
         <v>"Dying World"</v>
       </c>
       <c r="F48" s="1" t="str">
-        <f>CONCATENATE($C$1,A48," = ","{",$B$2," = ",B48,", ",$C$2," = ",E48,",",$G$2,G48,",",$H$2,H48,"}","")</f>
+        <f t="shared" si="5"/>
         <v>worldhooks[45] = {createworldcode = 41, text = "Dying World",x =755,y = 381}</v>
       </c>
       <c r="G48" s="1">
         <v>755</v>
       </c>
       <c r="H48" s="1">
-        <f>H47+$N$1</f>
+        <f t="shared" si="3"/>
         <v>381</v>
       </c>
       <c r="L48" s="1" t="s">
@@ -7190,18 +6674,18 @@
         <v>127</v>
       </c>
       <c r="E49" s="2" t="str">
-        <f>CONCATENATE(D49,C49,D49)</f>
+        <f t="shared" si="4"/>
         <v>"Enemies"</v>
       </c>
       <c r="F49" s="1" t="str">
-        <f>CONCATENATE($C$1,A49," = ","{",$B$2," = ",B49,", ",$C$2," = ",E49,",",$G$2,G49,",",$H$2,H49,"}","")</f>
+        <f t="shared" si="5"/>
         <v>worldhooks[46] = {createworldcode = 42, text = "Enemies",x =755,y = 396}</v>
       </c>
       <c r="G49" s="1">
         <v>755</v>
       </c>
       <c r="H49" s="1">
-        <f>H48+$N$1</f>
+        <f t="shared" si="3"/>
         <v>396</v>
       </c>
       <c r="L49" s="1" t="s">
@@ -7222,18 +6706,18 @@
         <v>127</v>
       </c>
       <c r="E50" s="2" t="str">
-        <f>CONCATENATE(D50,C50,D50)</f>
+        <f t="shared" si="4"/>
         <v>"Exploration"</v>
       </c>
       <c r="F50" s="1" t="str">
-        <f>CONCATENATE($C$1,A50," = ","{",$B$2," = ",B50,", ",$C$2," = ",E50,",",$G$2,G50,",",$H$2,H50,"}","")</f>
+        <f t="shared" si="5"/>
         <v>worldhooks[47] = {createworldcode = 43, text = "Exploration",x =755,y = 411}</v>
       </c>
       <c r="G50" s="1">
         <v>755</v>
       </c>
       <c r="H50" s="1">
-        <f>H49+$N$1</f>
+        <f t="shared" si="3"/>
         <v>411</v>
       </c>
       <c r="L50" s="1" t="s">
@@ -7254,18 +6738,18 @@
         <v>127</v>
       </c>
       <c r="E51" s="2" t="str">
-        <f>CONCATENATE(D51,C51,D51)</f>
+        <f t="shared" si="4"/>
         <v>"Frontier"</v>
       </c>
       <c r="F51" s="1" t="str">
-        <f>CONCATENATE($C$1,A51," = ","{",$B$2," = ",B51,", ",$C$2," = ",E51,",",$G$2,G51,",",$H$2,H51,"}","")</f>
+        <f t="shared" si="5"/>
         <v>worldhooks[48] = {createworldcode = 44, text = "Frontier",x =755,y = 426}</v>
       </c>
       <c r="G51" s="1">
         <v>755</v>
       </c>
       <c r="H51" s="1">
-        <f>H50+$N$1</f>
+        <f t="shared" si="3"/>
         <v>426</v>
       </c>
       <c r="L51" s="1" t="s">
@@ -7286,18 +6770,18 @@
         <v>127</v>
       </c>
       <c r="E52" s="2" t="str">
-        <f>CONCATENATE(D52,C52,D52)</f>
+        <f t="shared" si="4"/>
         <v>"Magical"</v>
       </c>
       <c r="F52" s="1" t="str">
-        <f>CONCATENATE($C$1,A52," = ","{",$B$2," = ",B52,", ",$C$2," = ",E52,",",$G$2,G52,",",$H$2,H52,"}","")</f>
+        <f t="shared" si="5"/>
         <v>worldhooks[49] = {createworldcode = 45, text = "Magical",x =755,y = 441}</v>
       </c>
       <c r="G52" s="1">
         <v>755</v>
       </c>
       <c r="H52" s="1">
-        <f>H51+$N$1</f>
+        <f t="shared" si="3"/>
         <v>441</v>
       </c>
       <c r="L52" s="1" t="s">
@@ -7318,18 +6802,18 @@
         <v>127</v>
       </c>
       <c r="E53" s="2" t="str">
-        <f>CONCATENATE(D53,C53,D53)</f>
+        <f t="shared" si="4"/>
         <v>"New World"</v>
       </c>
       <c r="F53" s="1" t="str">
-        <f>CONCATENATE($C$1,A53," = ","{",$B$2," = ",B53,", ",$C$2," = ",E53,",",$G$2,G53,",",$H$2,H53,"}","")</f>
+        <f t="shared" si="5"/>
         <v>worldhooks[50] = {createworldcode = 46, text = "New World",x =755,y = 456}</v>
       </c>
       <c r="G53" s="1">
         <v>755</v>
       </c>
       <c r="H53" s="1">
-        <f>H52+$N$1</f>
+        <f t="shared" si="3"/>
         <v>456</v>
       </c>
       <c r="L53" s="1" t="s">
@@ -7350,18 +6834,18 @@
         <v>127</v>
       </c>
       <c r="E54" s="2" t="str">
-        <f>CONCATENATE(D54,C54,D54)</f>
+        <f t="shared" si="4"/>
         <v>"Psionics"</v>
       </c>
       <c r="F54" s="1" t="str">
-        <f>CONCATENATE($C$1,A54," = ","{",$B$2," = ",B54,", ",$C$2," = ",E54,",",$G$2,G54,",",$H$2,H54,"}","")</f>
+        <f t="shared" si="5"/>
         <v>worldhooks[51] = {createworldcode = 47, text = "Psionics",x =755,y = 471}</v>
       </c>
       <c r="G54" s="1">
         <v>755</v>
       </c>
       <c r="H54" s="1">
-        <f>H53+$N$1</f>
+        <f t="shared" si="3"/>
         <v>471</v>
       </c>
       <c r="L54" s="1" t="s">
@@ -7382,18 +6866,18 @@
         <v>127</v>
       </c>
       <c r="E55" s="2" t="str">
-        <f>CONCATENATE(D55,C55,D55)</f>
+        <f t="shared" si="4"/>
         <v>"Race Dominance"</v>
       </c>
       <c r="F55" s="1" t="str">
-        <f>CONCATENATE($C$1,A55," = ","{",$B$2," = ",B55,", ",$C$2," = ",E55,",",$G$2,G55,",",$H$2,H55,"}","")</f>
+        <f t="shared" si="5"/>
         <v>worldhooks[52] = {createworldcode = 48, text = "Race Dominance",x =755,y = 486}</v>
       </c>
       <c r="G55" s="1">
         <v>755</v>
       </c>
       <c r="H55" s="1">
-        <f>H54+$N$1</f>
+        <f t="shared" si="3"/>
         <v>486</v>
       </c>
       <c r="L55" s="1" t="s">
@@ -7414,18 +6898,18 @@
         <v>127</v>
       </c>
       <c r="E56" s="2" t="str">
-        <f>CONCATENATE(D56,C56,D56)</f>
+        <f t="shared" si="4"/>
         <v>"Religious"</v>
       </c>
       <c r="F56" s="1" t="str">
-        <f>CONCATENATE($C$1,A56," = ","{",$B$2," = ",B56,", ",$C$2," = ",E56,",",$G$2,G56,",",$H$2,H56,"}","")</f>
+        <f t="shared" si="5"/>
         <v>worldhooks[53] = {createworldcode = 49, text = "Religious",x =755,y = 501}</v>
       </c>
       <c r="G56" s="1">
         <v>755</v>
       </c>
       <c r="H56" s="1">
-        <f>H55+$N$1</f>
+        <f t="shared" si="3"/>
         <v>501</v>
       </c>
       <c r="L56" s="1" t="s">
@@ -7446,18 +6930,18 @@
         <v>127</v>
       </c>
       <c r="E57" s="2" t="str">
-        <f>CONCATENATE(D57,C57,D57)</f>
+        <f t="shared" si="4"/>
         <v>"Slavery"</v>
       </c>
       <c r="F57" s="1" t="str">
-        <f>CONCATENATE($C$1,A57," = ","{",$B$2," = ",B57,", ",$C$2," = ",E57,",",$G$2,G57,",",$H$2,H57,"}","")</f>
+        <f t="shared" si="5"/>
         <v>worldhooks[54] = {createworldcode = 50, text = "Slavery",x =755,y = 516}</v>
       </c>
       <c r="G57" s="1">
         <v>755</v>
       </c>
       <c r="H57" s="1">
-        <f>H56+$N$1</f>
+        <f t="shared" si="3"/>
         <v>516</v>
       </c>
       <c r="L57" s="1" t="s">
@@ -7478,18 +6962,18 @@
         <v>127</v>
       </c>
       <c r="E58" s="2" t="str">
-        <f>CONCATENATE(D58,C58,D58)</f>
+        <f t="shared" si="4"/>
         <v>"Technology"</v>
       </c>
       <c r="F58" s="1" t="str">
-        <f>CONCATENATE($C$1,A58," = ","{",$B$2," = ",B58,", ",$C$2," = ",E58,",",$G$2,G58,",",$H$2,H58,"}","")</f>
+        <f t="shared" si="5"/>
         <v>worldhooks[55] = {createworldcode = 51, text = "Technology",x =755,y = 531}</v>
       </c>
       <c r="G58" s="1">
         <v>755</v>
       </c>
       <c r="H58" s="1">
-        <f>H57+$N$1</f>
+        <f t="shared" si="3"/>
         <v>531</v>
       </c>
       <c r="L58" s="1" t="s">
@@ -7510,18 +6994,18 @@
         <v>127</v>
       </c>
       <c r="E59" s="2" t="str">
-        <f>CONCATENATE(D59,C59,D59)</f>
+        <f t="shared" si="4"/>
         <v>"Warfare"</v>
       </c>
       <c r="F59" s="1" t="str">
-        <f>CONCATENATE($C$1,A59," = ","{",$B$2," = ",B59,", ",$C$2," = ",E59,",",$G$2,G59,",",$H$2,H59,"}","")</f>
+        <f t="shared" si="5"/>
         <v>worldhooks[56] = {createworldcode = 52, text = "Warfare",x =755,y = 546}</v>
       </c>
       <c r="G59" s="1">
         <v>755</v>
       </c>
       <c r="H59" s="1">
-        <f>H58+$N$1</f>
+        <f t="shared" si="3"/>
         <v>546</v>
       </c>
       <c r="L59" s="1" t="s">
@@ -7542,18 +7026,18 @@
         <v>127</v>
       </c>
       <c r="E60" s="2" t="str">
-        <f>CONCATENATE(D60,C60,D60)</f>
+        <f t="shared" si="4"/>
         <v>"Ancient Warfare"</v>
       </c>
       <c r="F60" s="1" t="str">
-        <f>CONCATENATE($C$1,A60," = ","{",$B$2," = ",B60,", ",$C$2," = ",E60,",",$G$2,G60,",",$H$2,H60,"}","")</f>
+        <f t="shared" si="5"/>
         <v>worldhooks[58] = {createworldcode = 53, text = "Ancient Warfare",x =1055,y = 561}</v>
       </c>
       <c r="G60" s="1">
         <v>1055</v>
       </c>
       <c r="H60" s="1">
-        <f>H59+$N$1</f>
+        <f t="shared" si="3"/>
         <v>561</v>
       </c>
       <c r="L60" s="1" t="s">
@@ -7574,18 +7058,18 @@
         <v>127</v>
       </c>
       <c r="E61" s="2" t="str">
-        <f>CONCATENATE(D61,C61,D61)</f>
+        <f t="shared" si="4"/>
         <v>"Artefact"</v>
       </c>
       <c r="F61" s="1" t="str">
-        <f>CONCATENATE($C$1,A61," = ","{",$B$2," = ",B61,", ",$C$2," = ",E61,",",$G$2,G61,",",$H$2,H61,"}","")</f>
+        <f t="shared" si="5"/>
         <v>worldhooks[59] = {createworldcode = 54, text = "Artefact",x =1055,y = 576}</v>
       </c>
       <c r="G61" s="1">
         <v>1055</v>
       </c>
       <c r="H61" s="1">
-        <f>H60+$N$1</f>
+        <f t="shared" si="3"/>
         <v>576</v>
       </c>
       <c r="L61" s="1" t="s">
@@ -7606,18 +7090,18 @@
         <v>127</v>
       </c>
       <c r="E62" s="2" t="str">
-        <f>CONCATENATE(D62,C62,D62)</f>
+        <f t="shared" si="4"/>
         <v>"Balkanisation"</v>
       </c>
       <c r="F62" s="1" t="str">
-        <f>CONCATENATE($C$1,A62," = ","{",$B$2," = ",B62,", ",$C$2," = ",E62,",",$G$2,G62,",",$H$2,H62,"}","")</f>
+        <f t="shared" si="5"/>
         <v>worldhooks[60] = {createworldcode = 55, text = "Balkanisation",x =1055,y = 591}</v>
       </c>
       <c r="G62" s="1">
         <v>1055</v>
       </c>
       <c r="H62" s="1">
-        <f>H61+$N$1</f>
+        <f t="shared" si="3"/>
         <v>591</v>
       </c>
       <c r="L62" s="1" t="s">
@@ -7638,18 +7122,18 @@
         <v>127</v>
       </c>
       <c r="E63" s="2" t="str">
-        <f>CONCATENATE(D63,C63,D63)</f>
+        <f t="shared" si="4"/>
         <v>"Civil War"</v>
       </c>
       <c r="F63" s="1" t="str">
-        <f>CONCATENATE($C$1,A63," = ","{",$B$2," = ",B63,", ",$C$2," = ",E63,",",$G$2,G63,",",$H$2,H63,"}","")</f>
+        <f t="shared" si="5"/>
         <v>worldhooks[61] = {createworldcode = 56, text = "Civil War",x =1055,y = 606}</v>
       </c>
       <c r="G63" s="1">
         <v>1055</v>
       </c>
       <c r="H63" s="1">
-        <f>H62+$N$1</f>
+        <f t="shared" si="3"/>
         <v>606</v>
       </c>
       <c r="L63" s="1" t="s">
@@ -7670,18 +7154,18 @@
         <v>127</v>
       </c>
       <c r="E64" s="2" t="str">
-        <f>CONCATENATE(D64,C64,D64)</f>
+        <f t="shared" si="4"/>
         <v>"Crusade"</v>
       </c>
       <c r="F64" s="1" t="str">
-        <f>CONCATENATE($C$1,A64," = ","{",$B$2," = ",B64,", ",$C$2," = ",E64,",",$G$2,G64,",",$H$2,H64,"}","")</f>
+        <f t="shared" si="5"/>
         <v>worldhooks[62] = {createworldcode = 57, text = "Crusade",x =1055,y = 621}</v>
       </c>
       <c r="G64" s="1">
         <v>1055</v>
       </c>
       <c r="H64" s="1">
-        <f>H63+$N$1</f>
+        <f t="shared" si="3"/>
         <v>621</v>
       </c>
       <c r="L64" s="1" t="s">
@@ -7702,18 +7186,18 @@
         <v>127</v>
       </c>
       <c r="E65" s="2" t="str">
-        <f>CONCATENATE(D65,C65,D65)</f>
+        <f t="shared" si="4"/>
         <v>"Insurrection"</v>
       </c>
       <c r="F65" s="1" t="str">
-        <f>CONCATENATE($C$1,A65," = ","{",$B$2," = ",B65,", ",$C$2," = ",E65,",",$G$2,G65,",",$H$2,H65,"}","")</f>
+        <f t="shared" si="5"/>
         <v>worldhooks[63] = {createworldcode = 58, text = "Insurrection",x =1055,y = 636}</v>
       </c>
       <c r="G65" s="1">
         <v>1055</v>
       </c>
       <c r="H65" s="1">
-        <f>H64+$N$1</f>
+        <f t="shared" si="3"/>
         <v>636</v>
       </c>
       <c r="L65" s="1" t="s">
@@ -7734,18 +7218,18 @@
         <v>127</v>
       </c>
       <c r="E66" s="2" t="str">
-        <f>CONCATENATE(D66,C66,D66)</f>
+        <f t="shared" si="4"/>
         <v>"Migration"</v>
       </c>
       <c r="F66" s="1" t="str">
-        <f>CONCATENATE($C$1,A66," = ","{",$B$2," = ",B66,", ",$C$2," = ",E66,",",$G$2,G66,",",$H$2,H66,"}","")</f>
+        <f t="shared" si="5"/>
         <v>worldhooks[64] = {createworldcode = 59, text = "Migration",x =1055,y = 651}</v>
       </c>
       <c r="G66" s="1">
         <v>1055</v>
       </c>
       <c r="H66" s="1">
-        <f>H65+$N$1</f>
+        <f t="shared" si="3"/>
         <v>651</v>
       </c>
       <c r="L66" s="1" t="s">
@@ -7766,18 +7250,18 @@
         <v>127</v>
       </c>
       <c r="E67" s="2" t="str">
-        <f>CONCATENATE(D67,C67,D67)</f>
+        <f t="shared" ref="E67:E98" si="6">CONCATENATE(D67,C67,D67)</f>
         <v>"Post Apocalyptic"</v>
       </c>
       <c r="F67" s="1" t="str">
-        <f>CONCATENATE($C$1,A67," = ","{",$B$2," = ",B67,", ",$C$2," = ",E67,",",$G$2,G67,",",$H$2,H67,"}","")</f>
+        <f t="shared" ref="F67:F98" si="7">CONCATENATE($C$1,A67," = ","{",$B$2," = ",B67,", ",$C$2," = ",E67,",",$G$2,G67,",",$H$2,H67,"}","")</f>
         <v>worldhooks[65] = {createworldcode = 60, text = "Post Apocalyptic",x =1055,y = 666}</v>
       </c>
       <c r="G67" s="1">
         <v>1055</v>
       </c>
       <c r="H67" s="1">
-        <f>H66+$N$1</f>
+        <f t="shared" si="3"/>
         <v>666</v>
       </c>
       <c r="L67" s="1" t="s">
@@ -7799,4 +7283,568 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O29" sqref="O29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F1" t="s">
+        <v>137</v>
+      </c>
+      <c r="J1" t="s">
+        <v>135</v>
+      </c>
+      <c r="K1" t="s">
+        <v>136</v>
+      </c>
+      <c r="L1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F2" t="s">
+        <v>138</v>
+      </c>
+      <c r="G2" t="s">
+        <v>139</v>
+      </c>
+      <c r="J2" t="s">
+        <v>208</v>
+      </c>
+      <c r="K2" t="s">
+        <v>208</v>
+      </c>
+      <c r="L2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>800</v>
+      </c>
+      <c r="C3">
+        <v>1287.4752000000001</v>
+      </c>
+      <c r="D3">
+        <v>50</v>
+      </c>
+      <c r="E3">
+        <v>80.467200000000005</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>16.093440000000001</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3" t="str">
+        <f>CONCATENATE(C3," ( ",B3," )")</f>
+        <v>1287.4752 ( 800 )</v>
+      </c>
+      <c r="K3" t="str">
+        <f>CONCATENATE(E3," ( ",D3," )")</f>
+        <v>80.4672 ( 50 )</v>
+      </c>
+      <c r="L3" t="str">
+        <f>CONCATENATE(G3," ( ",F3," )")</f>
+        <v>16.09344 ( 10 )</v>
+      </c>
+      <c r="N3" t="e">
+        <f>conc</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1600</v>
+      </c>
+      <c r="C4">
+        <v>2574.9504000000002</v>
+      </c>
+      <c r="D4">
+        <v>100</v>
+      </c>
+      <c r="E4">
+        <v>160.93440000000001</v>
+      </c>
+      <c r="F4">
+        <v>20</v>
+      </c>
+      <c r="G4">
+        <v>32.186880000000002</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" ref="J4:J11" si="0">CONCATENATE(C4," ( ",B4," )")</f>
+        <v>2574.9504 ( 1600 )</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" ref="K4:K11" si="1">CONCATENATE(E4," ( ",D4," )")</f>
+        <v>160.9344 ( 100 )</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" ref="L4:L11" si="2">CONCATENATE(G4," ( ",F4," )")</f>
+        <v>32.18688 ( 20 )</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>2400</v>
+      </c>
+      <c r="C5">
+        <v>3862.4256000000005</v>
+      </c>
+      <c r="D5">
+        <v>150</v>
+      </c>
+      <c r="E5">
+        <v>241.40160000000003</v>
+      </c>
+      <c r="F5">
+        <v>30</v>
+      </c>
+      <c r="G5">
+        <v>48.280320000000003</v>
+      </c>
+      <c r="I5">
+        <v>3</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="0"/>
+        <v>3862.4256 ( 2400 )</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="1"/>
+        <v>241.4016 ( 150 )</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="2"/>
+        <v>48.28032 ( 30 )</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>4000</v>
+      </c>
+      <c r="C6">
+        <v>6437.3760000000002</v>
+      </c>
+      <c r="D6">
+        <v>250</v>
+      </c>
+      <c r="E6">
+        <v>402.33600000000001</v>
+      </c>
+      <c r="F6">
+        <v>50</v>
+      </c>
+      <c r="G6">
+        <v>80.467200000000005</v>
+      </c>
+      <c r="I6">
+        <v>4</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="0"/>
+        <v>6437.376 ( 4000 )</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="1"/>
+        <v>402.336 ( 250 )</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="2"/>
+        <v>80.4672 ( 50 )</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>4800</v>
+      </c>
+      <c r="C7">
+        <v>7724.851200000001</v>
+      </c>
+      <c r="D7">
+        <v>300</v>
+      </c>
+      <c r="E7">
+        <v>482.80320000000006</v>
+      </c>
+      <c r="F7">
+        <v>60</v>
+      </c>
+      <c r="G7">
+        <v>96.560640000000006</v>
+      </c>
+      <c r="I7">
+        <v>5</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="0"/>
+        <v>7724.8512 ( 4800 )</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="1"/>
+        <v>482.8032 ( 300 )</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="2"/>
+        <v>96.56064 ( 60 )</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>8000</v>
+      </c>
+      <c r="C8">
+        <v>12874.752</v>
+      </c>
+      <c r="D8">
+        <v>500</v>
+      </c>
+      <c r="E8">
+        <v>804.67200000000003</v>
+      </c>
+      <c r="F8">
+        <v>100</v>
+      </c>
+      <c r="G8">
+        <v>160.93440000000001</v>
+      </c>
+      <c r="I8">
+        <v>6</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="0"/>
+        <v>12874.752 ( 8000 )</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="1"/>
+        <v>804.672 ( 500 )</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="2"/>
+        <v>160.9344 ( 100 )</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>10000</v>
+      </c>
+      <c r="C9">
+        <v>16093.44</v>
+      </c>
+      <c r="D9">
+        <v>625</v>
+      </c>
+      <c r="E9">
+        <v>1005.84</v>
+      </c>
+      <c r="F9">
+        <v>125</v>
+      </c>
+      <c r="G9">
+        <v>201.16800000000001</v>
+      </c>
+      <c r="I9">
+        <v>7</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="0"/>
+        <v>16093.44 ( 10000 )</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="1"/>
+        <v>1005.84 ( 625 )</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="2"/>
+        <v>201.168 ( 125 )</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>12000</v>
+      </c>
+      <c r="C10">
+        <v>19312.128000000001</v>
+      </c>
+      <c r="D10">
+        <v>750</v>
+      </c>
+      <c r="E10">
+        <v>1207.008</v>
+      </c>
+      <c r="F10">
+        <v>150</v>
+      </c>
+      <c r="G10">
+        <v>241.40160000000003</v>
+      </c>
+      <c r="I10">
+        <v>8</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="0"/>
+        <v>19312.128 ( 12000 )</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="1"/>
+        <v>1207.008 ( 750 )</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="2"/>
+        <v>241.4016 ( 150 )</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>16000</v>
+      </c>
+      <c r="C11">
+        <v>25749.504000000001</v>
+      </c>
+      <c r="D11">
+        <v>1000</v>
+      </c>
+      <c r="E11">
+        <v>1609.3440000000001</v>
+      </c>
+      <c r="F11">
+        <v>200</v>
+      </c>
+      <c r="G11">
+        <v>321.86880000000002</v>
+      </c>
+      <c r="I11">
+        <v>9</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="0"/>
+        <v>25749.504 ( 16000 )</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="1"/>
+        <v>1609.344 ( 1000 )</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="2"/>
+        <v>321.8688 ( 200 )</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J13" t="s">
+        <v>135</v>
+      </c>
+      <c r="K13" t="s">
+        <v>136</v>
+      </c>
+      <c r="L13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J14" t="s">
+        <v>208</v>
+      </c>
+      <c r="K14" t="s">
+        <v>208</v>
+      </c>
+      <c r="L14" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="L15" s="7" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <v>2</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="L16" s="7" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="17" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>3</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="L17" s="7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="18" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <v>4</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="L18" s="7" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="19" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>5</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="K19" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="L19" s="7" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="20" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <v>6</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="K20" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="L20" s="7" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="21" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <v>7</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="K21" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="L21" s="7" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="22" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <v>8</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="K22" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="L22" s="7" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="23" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="I23">
+        <v>9</v>
+      </c>
+      <c r="J23" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="K23" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="L23" s="7" t="s">
+        <v>232</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>